<commit_message>
correcting body fat percentage method and retirement
</commit_message>
<xml_diff>
--- a/data_processing_elements-HBS.xlsx
+++ b/data_processing_elements-HBS.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maelstrom\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbtiali\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8F14FDC-3B98-47F2-9579-0BC8BD74D3DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF4A06D3-38E5-4AEA-BE30-12A292C1CA68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{A2851C76-6816-460F-844D-5B34B01F8802}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A2851C76-6816-460F-844D-5B34B01F8802}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -477,11 +477,6 @@
 1 = Retired</t>
   </si>
   <si>
-    <t>case_when(
-LIS05b_situations_pursuits_most == 9 ~ 1L;
-ELSE ~ 0L)</t>
-  </si>
-  <si>
     <t>participants are between 30-39 so there should not be any retired person</t>
   </si>
   <si>
@@ -669,11 +664,6 @@
   </si>
   <si>
     <t>Method used to measure the body fat percentage</t>
-  </si>
-  <si>
-    <t>case_when(
-!is.na(BOD104_waist_circumference_rounded) ~ "Bioelectrical impedance measurement (Bodystat Multi-Scan 5000)";
-ELSE ~ NA_character_)</t>
   </si>
   <si>
     <t>pm_systo_bp</t>
@@ -1556,6 +1546,17 @@
   </si>
   <si>
     <t>as.integer(as.numeric(SBQ_total)/7)</t>
+  </si>
+  <si>
+    <t>case_when(
+!is.na(BOD109_fat_percentage) ~ "Bioelectrical impedance measurement (Bodystat Multi-Scan 5000)";
+ELSE ~ NA_character_)</t>
+  </si>
+  <si>
+    <t>case_when(
+LIS05b_situations_pursuits_most == 9 ~ 1L;
+LIS05b_situations_pursuits_most %in% c(1:8,10:14) ~ 0L;
+ELSE ~ NA)</t>
   </si>
 </sst>
 </file>
@@ -1941,13 +1942,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1AF92DA-191C-4FF7-9A4B-8BE07EA34827}">
   <dimension ref="A1:AD84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L76" workbookViewId="0">
-      <selection activeCell="T76" sqref="T76"/>
+    <sheetView tabSelected="1" topLeftCell="S11" workbookViewId="0">
+      <selection activeCell="W13" sqref="W13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="54.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2039,7 +2040,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2083,7 +2084,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2136,7 +2137,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:30" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:30" ht="30" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2180,7 +2181,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:30" ht="377" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:30" ht="60" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2221,7 +2222,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="6" spans="1:30" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:30" ht="180" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2244,7 +2245,7 @@
         <v>71</v>
       </c>
       <c r="J6" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="M6" t="s">
         <v>72</v>
@@ -2280,7 +2281,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:30" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:30" ht="105" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2321,7 +2322,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:30" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:30" ht="240" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2365,7 +2366,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="9" spans="1:30" ht="261" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:30" ht="60" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2409,7 +2410,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2450,7 +2451,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:30" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:30" ht="390" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2494,7 +2495,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="12" spans="1:30" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:30" ht="240" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2535,13 +2536,13 @@
         <v>101</v>
       </c>
       <c r="W12" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="X12" t="s">
         <v>118</v>
       </c>
-      <c r="X12" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="13" spans="1:30" ht="159.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:30" ht="75" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2549,28 +2550,28 @@
         <v>30</v>
       </c>
       <c r="C13" t="s">
+        <v>119</v>
+      </c>
+      <c r="D13" t="s">
         <v>120</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>121</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
+        <v>56</v>
+      </c>
+      <c r="I13" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="F13" t="s">
-        <v>56</v>
-      </c>
-      <c r="I13" s="1" t="s">
+      <c r="J13" t="s">
         <v>123</v>
       </c>
-      <c r="J13" t="s">
+      <c r="M13" t="s">
         <v>124</v>
       </c>
-      <c r="M13" t="s">
+      <c r="Q13" s="1" t="s">
         <v>125</v>
-      </c>
-      <c r="Q13" s="1" t="s">
-        <v>126</v>
       </c>
       <c r="T13" t="s">
         <v>36</v>
@@ -2582,10 +2583,10 @@
         <v>60</v>
       </c>
       <c r="W13" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="14" spans="1:30" ht="101.5" x14ac:dyDescent="0.35">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" ht="30" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2593,19 +2594,19 @@
         <v>30</v>
       </c>
       <c r="C14" t="s">
+        <v>127</v>
+      </c>
+      <c r="D14" t="s">
         <v>128</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>129</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
+        <v>56</v>
+      </c>
+      <c r="I14" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="F14" t="s">
-        <v>56</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>131</v>
       </c>
       <c r="J14" t="s">
         <v>47</v>
@@ -2623,7 +2624,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="15" spans="1:30" ht="29" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:30" ht="30" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2631,25 +2632,25 @@
         <v>30</v>
       </c>
       <c r="C15" t="s">
+        <v>131</v>
+      </c>
+      <c r="D15" t="s">
         <v>132</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
+        <v>132</v>
+      </c>
+      <c r="F15" t="s">
+        <v>56</v>
+      </c>
+      <c r="I15" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="E15" t="s">
-        <v>133</v>
-      </c>
-      <c r="F15" t="s">
-        <v>56</v>
-      </c>
-      <c r="I15" s="1" t="s">
+      <c r="J15" t="s">
         <v>134</v>
       </c>
-      <c r="J15" t="s">
+      <c r="K15" t="s">
         <v>135</v>
-      </c>
-      <c r="K15" t="s">
-        <v>136</v>
       </c>
       <c r="T15" t="s">
         <v>48</v>
@@ -2664,16 +2665,16 @@
         <v>48</v>
       </c>
       <c r="X15" t="s">
+        <v>136</v>
+      </c>
+      <c r="AA15" t="s">
         <v>137</v>
-      </c>
-      <c r="AA15" t="s">
-        <v>138</v>
       </c>
       <c r="AB15" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2681,28 +2682,28 @@
         <v>30</v>
       </c>
       <c r="C16" t="s">
+        <v>138</v>
+      </c>
+      <c r="D16" t="s">
         <v>139</v>
       </c>
-      <c r="D16" t="s">
-        <v>140</v>
-      </c>
       <c r="E16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F16" t="s">
         <v>106</v>
       </c>
       <c r="G16" t="s">
+        <v>140</v>
+      </c>
+      <c r="J16" t="s">
         <v>141</v>
       </c>
-      <c r="J16" t="s">
+      <c r="K16" t="s">
         <v>142</v>
       </c>
-      <c r="K16" t="s">
-        <v>143</v>
-      </c>
       <c r="R16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="T16" t="s">
         <v>36</v>
@@ -2717,13 +2718,13 @@
         <v>67</v>
       </c>
       <c r="AA16" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="AB16" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:28" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:28" ht="45" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2731,22 +2732,22 @@
         <v>30</v>
       </c>
       <c r="C17" t="s">
+        <v>144</v>
+      </c>
+      <c r="D17" t="s">
         <v>145</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
+        <v>145</v>
+      </c>
+      <c r="F17" t="s">
+        <v>56</v>
+      </c>
+      <c r="I17" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="E17" t="s">
-        <v>146</v>
-      </c>
-      <c r="F17" t="s">
-        <v>56</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>147</v>
-      </c>
       <c r="J17" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="T17" t="s">
         <v>36</v>
@@ -2758,16 +2759,16 @@
         <v>101</v>
       </c>
       <c r="W17" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="AA17" t="s">
         <v>148</v>
-      </c>
-      <c r="AA17" t="s">
-        <v>149</v>
       </c>
       <c r="AB17" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2775,28 +2776,28 @@
         <v>30</v>
       </c>
       <c r="C18" t="s">
+        <v>149</v>
+      </c>
+      <c r="D18" t="s">
         <v>150</v>
       </c>
-      <c r="D18" t="s">
-        <v>151</v>
-      </c>
       <c r="E18" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F18" t="s">
         <v>106</v>
       </c>
       <c r="G18" t="s">
+        <v>151</v>
+      </c>
+      <c r="J18" t="s">
         <v>152</v>
       </c>
-      <c r="J18" t="s">
+      <c r="K18" t="s">
         <v>153</v>
       </c>
-      <c r="K18" t="s">
-        <v>154</v>
-      </c>
       <c r="R18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="T18" t="s">
         <v>36</v>
@@ -2811,7 +2812,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="19" spans="1:28" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:28" ht="45" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2819,22 +2820,22 @@
         <v>30</v>
       </c>
       <c r="C19" t="s">
+        <v>154</v>
+      </c>
+      <c r="D19" t="s">
         <v>155</v>
       </c>
-      <c r="D19" t="s">
-        <v>156</v>
-      </c>
       <c r="E19" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F19" t="s">
         <v>56</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J19" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="T19" t="s">
         <v>36</v>
@@ -2846,16 +2847,16 @@
         <v>101</v>
       </c>
       <c r="W19" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AA19" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="AB19" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2863,28 +2864,28 @@
         <v>30</v>
       </c>
       <c r="C20" t="s">
+        <v>157</v>
+      </c>
+      <c r="D20" t="s">
         <v>158</v>
       </c>
-      <c r="D20" t="s">
-        <v>159</v>
-      </c>
       <c r="E20" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F20" t="s">
         <v>106</v>
       </c>
       <c r="G20" t="s">
+        <v>159</v>
+      </c>
+      <c r="J20" t="s">
         <v>160</v>
       </c>
-      <c r="J20" t="s">
+      <c r="K20" t="s">
         <v>161</v>
       </c>
-      <c r="K20" t="s">
-        <v>162</v>
-      </c>
       <c r="R20" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="T20" t="s">
         <v>36</v>
@@ -2899,7 +2900,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2907,28 +2908,28 @@
         <v>30</v>
       </c>
       <c r="C21" t="s">
+        <v>162</v>
+      </c>
+      <c r="D21" t="s">
         <v>163</v>
       </c>
-      <c r="D21" t="s">
-        <v>164</v>
-      </c>
       <c r="E21" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F21" t="s">
         <v>106</v>
       </c>
       <c r="G21" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J21" t="s">
+        <v>164</v>
+      </c>
+      <c r="K21" t="s">
         <v>165</v>
       </c>
-      <c r="K21" t="s">
-        <v>166</v>
-      </c>
       <c r="R21" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="T21" t="s">
         <v>36</v>
@@ -2943,13 +2944,13 @@
         <v>67</v>
       </c>
       <c r="AA21" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="AB21" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:28" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:28" ht="45" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2957,22 +2958,22 @@
         <v>30</v>
       </c>
       <c r="C22" t="s">
+        <v>167</v>
+      </c>
+      <c r="D22" t="s">
         <v>168</v>
       </c>
-      <c r="D22" t="s">
-        <v>169</v>
-      </c>
       <c r="E22" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F22" t="s">
         <v>56</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J22" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="T22" t="s">
         <v>36</v>
@@ -2984,10 +2985,10 @@
         <v>101</v>
       </c>
       <c r="W22" s="1" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.35">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2995,28 +2996,28 @@
         <v>30</v>
       </c>
       <c r="C23" t="s">
+        <v>170</v>
+      </c>
+      <c r="D23" t="s">
         <v>171</v>
       </c>
-      <c r="D23" t="s">
-        <v>172</v>
-      </c>
       <c r="E23" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F23" t="s">
         <v>106</v>
       </c>
       <c r="G23" t="s">
+        <v>172</v>
+      </c>
+      <c r="J23" t="s">
         <v>173</v>
       </c>
-      <c r="J23" t="s">
-        <v>174</v>
-      </c>
       <c r="K23" t="s">
+        <v>171</v>
+      </c>
+      <c r="R23" t="s">
         <v>172</v>
-      </c>
-      <c r="R23" t="s">
-        <v>173</v>
       </c>
       <c r="T23" t="s">
         <v>36</v>
@@ -3031,7 +3032,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="24" spans="1:28" ht="304.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:28" ht="60" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3039,19 +3040,19 @@
         <v>30</v>
       </c>
       <c r="C24" t="s">
+        <v>174</v>
+      </c>
+      <c r="D24" t="s">
         <v>175</v>
       </c>
-      <c r="D24" t="s">
-        <v>176</v>
-      </c>
       <c r="E24" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F24" t="s">
         <v>34</v>
       </c>
       <c r="J24" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="T24" t="s">
         <v>36</v>
@@ -3063,10 +3064,10 @@
         <v>101</v>
       </c>
       <c r="W24" s="1" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.35">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3074,28 +3075,28 @@
         <v>30</v>
       </c>
       <c r="C25" t="s">
+        <v>176</v>
+      </c>
+      <c r="D25" t="s">
+        <v>177</v>
+      </c>
+      <c r="E25" t="s">
         <v>178</v>
       </c>
-      <c r="D25" t="s">
+      <c r="F25" t="s">
+        <v>56</v>
+      </c>
+      <c r="G25" t="s">
         <v>179</v>
       </c>
-      <c r="E25" t="s">
+      <c r="J25" t="s">
         <v>180</v>
       </c>
-      <c r="F25" t="s">
-        <v>56</v>
-      </c>
-      <c r="G25" t="s">
+      <c r="K25" t="s">
         <v>181</v>
       </c>
-      <c r="J25" t="s">
-        <v>182</v>
-      </c>
-      <c r="K25" t="s">
-        <v>183</v>
-      </c>
       <c r="R25" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="T25" t="s">
         <v>36</v>
@@ -3110,7 +3111,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3118,28 +3119,28 @@
         <v>30</v>
       </c>
       <c r="C26" t="s">
+        <v>182</v>
+      </c>
+      <c r="D26" t="s">
+        <v>183</v>
+      </c>
+      <c r="E26" t="s">
         <v>184</v>
       </c>
-      <c r="D26" t="s">
+      <c r="F26" t="s">
+        <v>56</v>
+      </c>
+      <c r="G26" t="s">
+        <v>179</v>
+      </c>
+      <c r="J26" t="s">
         <v>185</v>
       </c>
-      <c r="E26" t="s">
+      <c r="K26" t="s">
         <v>186</v>
       </c>
-      <c r="F26" t="s">
-        <v>56</v>
-      </c>
-      <c r="G26" t="s">
-        <v>181</v>
-      </c>
-      <c r="J26" t="s">
-        <v>187</v>
-      </c>
-      <c r="K26" t="s">
-        <v>188</v>
-      </c>
       <c r="R26" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="T26" t="s">
         <v>36</v>
@@ -3154,7 +3155,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="27" spans="1:28" ht="406" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:28" ht="90" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3162,28 +3163,28 @@
         <v>30</v>
       </c>
       <c r="C27" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D27" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E27" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F27" t="s">
         <v>106</v>
       </c>
       <c r="G27" t="s">
+        <v>189</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="K27" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="J27" s="1" t="s">
+      <c r="R27" t="s">
         <v>192</v>
-      </c>
-      <c r="K27" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="R27" t="s">
-        <v>194</v>
       </c>
       <c r="T27" t="s">
         <v>48</v>
@@ -3198,10 +3199,10 @@
         <v>48</v>
       </c>
       <c r="X27" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.35">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3209,25 +3210,25 @@
         <v>30</v>
       </c>
       <c r="C28" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D28" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E28" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F28" t="s">
         <v>106</v>
       </c>
       <c r="G28" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="J28" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="S28" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="T28" t="s">
         <v>36</v>
@@ -3242,10 +3243,10 @@
         <v>67</v>
       </c>
       <c r="X28" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="29" spans="1:28" ht="101.5" x14ac:dyDescent="0.35">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="29" spans="1:28" ht="45" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3253,22 +3254,22 @@
         <v>30</v>
       </c>
       <c r="C29" t="s">
+        <v>200</v>
+      </c>
+      <c r="D29" t="s">
+        <v>201</v>
+      </c>
+      <c r="E29" t="s">
+        <v>201</v>
+      </c>
+      <c r="F29" t="s">
+        <v>56</v>
+      </c>
+      <c r="I29" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="D29" t="s">
+      <c r="J29" t="s">
         <v>203</v>
-      </c>
-      <c r="E29" t="s">
-        <v>203</v>
-      </c>
-      <c r="F29" t="s">
-        <v>56</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="J29" t="s">
-        <v>205</v>
       </c>
       <c r="T29" t="s">
         <v>48</v>
@@ -3283,7 +3284,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3291,28 +3292,28 @@
         <v>30</v>
       </c>
       <c r="C30" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D30" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E30" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F30" t="s">
         <v>106</v>
       </c>
       <c r="G30" t="s">
+        <v>206</v>
+      </c>
+      <c r="J30" t="s">
+        <v>207</v>
+      </c>
+      <c r="K30" t="s">
         <v>208</v>
       </c>
-      <c r="J30" t="s">
-        <v>209</v>
-      </c>
-      <c r="K30" t="s">
-        <v>210</v>
-      </c>
       <c r="R30" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="T30" t="s">
         <v>36</v>
@@ -3327,7 +3328,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -3335,19 +3336,19 @@
         <v>30</v>
       </c>
       <c r="C31" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D31" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E31" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="F31" t="s">
         <v>106</v>
       </c>
       <c r="G31" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="J31" t="s">
         <v>47</v>
@@ -3365,7 +3366,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -3373,19 +3374,19 @@
         <v>30</v>
       </c>
       <c r="C32" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D32" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="E32" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F32" t="s">
         <v>106</v>
       </c>
       <c r="G32" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="J32" t="s">
         <v>47</v>
@@ -3403,7 +3404,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -3411,19 +3412,19 @@
         <v>30</v>
       </c>
       <c r="C33" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D33" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E33" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="F33" t="s">
         <v>106</v>
       </c>
       <c r="G33" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="J33" t="s">
         <v>47</v>
@@ -3441,7 +3442,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -3449,19 +3450,19 @@
         <v>30</v>
       </c>
       <c r="C34" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D34" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E34" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="F34" t="s">
         <v>106</v>
       </c>
       <c r="G34" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="J34" t="s">
         <v>47</v>
@@ -3479,7 +3480,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -3487,19 +3488,19 @@
         <v>30</v>
       </c>
       <c r="C35" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D35" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E35" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="F35" t="s">
         <v>106</v>
       </c>
       <c r="G35" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="J35" t="s">
         <v>47</v>
@@ -3517,7 +3518,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -3525,19 +3526,19 @@
         <v>30</v>
       </c>
       <c r="C36" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D36" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E36" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F36" t="s">
         <v>106</v>
       </c>
       <c r="G36" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="J36" t="s">
         <v>47</v>
@@ -3555,7 +3556,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="37" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -3563,19 +3564,19 @@
         <v>30</v>
       </c>
       <c r="C37" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D37" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E37" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="F37" t="s">
         <v>106</v>
       </c>
       <c r="G37" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="J37" t="s">
         <v>47</v>
@@ -3593,7 +3594,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="38" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -3601,19 +3602,19 @@
         <v>30</v>
       </c>
       <c r="C38" t="s">
+        <v>226</v>
+      </c>
+      <c r="D38" t="s">
+        <v>227</v>
+      </c>
+      <c r="E38" t="s">
         <v>228</v>
-      </c>
-      <c r="D38" t="s">
-        <v>229</v>
-      </c>
-      <c r="E38" t="s">
-        <v>230</v>
       </c>
       <c r="F38" t="s">
         <v>106</v>
       </c>
       <c r="G38" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="J38" t="s">
         <v>47</v>
@@ -3631,7 +3632,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="39" spans="1:28" ht="116" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:28" ht="45" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -3639,19 +3640,19 @@
         <v>30</v>
       </c>
       <c r="C39" t="s">
+        <v>230</v>
+      </c>
+      <c r="D39" t="s">
+        <v>231</v>
+      </c>
+      <c r="E39" t="s">
         <v>232</v>
       </c>
-      <c r="D39" t="s">
+      <c r="F39" t="s">
+        <v>56</v>
+      </c>
+      <c r="I39" s="1" t="s">
         <v>233</v>
-      </c>
-      <c r="E39" t="s">
-        <v>234</v>
-      </c>
-      <c r="F39" t="s">
-        <v>56</v>
-      </c>
-      <c r="I39" s="1" t="s">
-        <v>235</v>
       </c>
       <c r="J39" t="s">
         <v>47</v>
@@ -3669,7 +3670,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="40" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -3677,19 +3678,19 @@
         <v>30</v>
       </c>
       <c r="C40" t="s">
+        <v>234</v>
+      </c>
+      <c r="D40" t="s">
+        <v>235</v>
+      </c>
+      <c r="E40" t="s">
         <v>236</v>
-      </c>
-      <c r="D40" t="s">
-        <v>237</v>
-      </c>
-      <c r="E40" t="s">
-        <v>238</v>
       </c>
       <c r="F40" t="s">
         <v>106</v>
       </c>
       <c r="G40" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="J40" t="s">
         <v>47</v>
@@ -3707,7 +3708,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="41" spans="1:28" ht="116" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:28" ht="45" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -3715,19 +3716,19 @@
         <v>30</v>
       </c>
       <c r="C41" t="s">
+        <v>237</v>
+      </c>
+      <c r="D41" t="s">
+        <v>238</v>
+      </c>
+      <c r="E41" t="s">
         <v>239</v>
       </c>
-      <c r="D41" t="s">
-        <v>240</v>
-      </c>
-      <c r="E41" t="s">
-        <v>241</v>
-      </c>
       <c r="F41" t="s">
         <v>56</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="J41" t="s">
         <v>47</v>
@@ -3745,7 +3746,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="42" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -3753,19 +3754,19 @@
         <v>30</v>
       </c>
       <c r="C42" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D42" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="E42" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="F42" t="s">
         <v>106</v>
       </c>
       <c r="G42" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="J42" t="s">
         <v>47</v>
@@ -3783,13 +3784,13 @@
         <v>84</v>
       </c>
       <c r="AA42" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="AB42" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:28" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:28" ht="135" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -3797,31 +3798,31 @@
         <v>30</v>
       </c>
       <c r="C43" t="s">
+        <v>244</v>
+      </c>
+      <c r="D43" t="s">
+        <v>245</v>
+      </c>
+      <c r="E43" t="s">
         <v>246</v>
-      </c>
-      <c r="D43" t="s">
-        <v>247</v>
-      </c>
-      <c r="E43" t="s">
-        <v>248</v>
       </c>
       <c r="F43" t="s">
         <v>106</v>
       </c>
       <c r="G43" t="s">
+        <v>247</v>
+      </c>
+      <c r="J43" t="s">
+        <v>248</v>
+      </c>
+      <c r="K43" t="s">
         <v>249</v>
       </c>
-      <c r="J43" t="s">
+      <c r="Q43" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="K43" t="s">
+      <c r="S43" s="1" t="s">
         <v>251</v>
-      </c>
-      <c r="Q43" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="S43" s="1" t="s">
-        <v>253</v>
       </c>
       <c r="T43" t="s">
         <v>36</v>
@@ -3833,16 +3834,16 @@
         <v>101</v>
       </c>
       <c r="W43" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="AA43" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="AB43" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:28" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:28" ht="105" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -3850,25 +3851,25 @@
         <v>30</v>
       </c>
       <c r="C44" t="s">
+        <v>254</v>
+      </c>
+      <c r="D44" t="s">
+        <v>255</v>
+      </c>
+      <c r="E44" t="s">
+        <v>255</v>
+      </c>
+      <c r="F44" t="s">
+        <v>56</v>
+      </c>
+      <c r="I44" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="D44" t="s">
+      <c r="J44" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="E44" t="s">
-        <v>257</v>
-      </c>
-      <c r="F44" t="s">
-        <v>56</v>
-      </c>
-      <c r="I44" s="1" t="s">
+      <c r="Q44" s="1" t="s">
         <v>258</v>
-      </c>
-      <c r="J44" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="Q44" s="1" t="s">
-        <v>260</v>
       </c>
       <c r="T44" t="s">
         <v>36</v>
@@ -3880,10 +3881,10 @@
         <v>101</v>
       </c>
       <c r="W44" s="1" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="45" spans="1:28" ht="391.5" x14ac:dyDescent="0.35">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="45" spans="1:28" ht="120" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -3891,28 +3892,28 @@
         <v>30</v>
       </c>
       <c r="C45" t="s">
+        <v>260</v>
+      </c>
+      <c r="D45" t="s">
+        <v>261</v>
+      </c>
+      <c r="E45" t="s">
         <v>262</v>
       </c>
-      <c r="D45" t="s">
+      <c r="F45" t="s">
+        <v>56</v>
+      </c>
+      <c r="I45" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="E45" t="s">
+      <c r="J45" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="F45" t="s">
-        <v>56</v>
-      </c>
-      <c r="I45" s="1" t="s">
+      <c r="K45" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="J45" s="1" t="s">
+      <c r="Q45" s="1" t="s">
         <v>266</v>
-      </c>
-      <c r="K45" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="Q45" s="1" t="s">
-        <v>268</v>
       </c>
       <c r="T45" t="s">
         <v>48</v>
@@ -3927,10 +3928,10 @@
         <v>48</v>
       </c>
       <c r="X45" s="1" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="46" spans="1:28" ht="409.5" x14ac:dyDescent="0.35">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="46" spans="1:28" ht="150" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -3938,28 +3939,28 @@
         <v>30</v>
       </c>
       <c r="C46" t="s">
+        <v>268</v>
+      </c>
+      <c r="D46" t="s">
+        <v>269</v>
+      </c>
+      <c r="E46" t="s">
+        <v>269</v>
+      </c>
+      <c r="F46" t="s">
+        <v>56</v>
+      </c>
+      <c r="I46" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="D46" t="s">
+      <c r="J46" t="s">
         <v>271</v>
       </c>
-      <c r="E46" t="s">
-        <v>271</v>
-      </c>
-      <c r="F46" t="s">
-        <v>56</v>
-      </c>
-      <c r="I46" s="1" t="s">
+      <c r="K46" t="s">
         <v>272</v>
       </c>
-      <c r="J46" t="s">
+      <c r="Q46" s="1" t="s">
         <v>273</v>
-      </c>
-      <c r="K46" t="s">
-        <v>274</v>
-      </c>
-      <c r="Q46" s="1" t="s">
-        <v>275</v>
       </c>
       <c r="T46" t="s">
         <v>36</v>
@@ -3971,13 +3972,13 @@
         <v>60</v>
       </c>
       <c r="W46" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="X46" s="1" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="47" spans="1:28" ht="409.5" x14ac:dyDescent="0.35">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="47" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -3985,25 +3986,25 @@
         <v>30</v>
       </c>
       <c r="C47" t="s">
+        <v>276</v>
+      </c>
+      <c r="D47" t="s">
+        <v>277</v>
+      </c>
+      <c r="E47" t="s">
+        <v>277</v>
+      </c>
+      <c r="F47" t="s">
+        <v>56</v>
+      </c>
+      <c r="G47" t="s">
         <v>278</v>
       </c>
-      <c r="D47" t="s">
+      <c r="J47" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="E47" t="s">
-        <v>279</v>
-      </c>
-      <c r="F47" t="s">
-        <v>56</v>
-      </c>
-      <c r="G47" t="s">
+      <c r="K47" s="1" t="s">
         <v>280</v>
-      </c>
-      <c r="J47" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="K47" s="1" t="s">
-        <v>282</v>
       </c>
       <c r="T47" t="s">
         <v>36</v>
@@ -4015,10 +4016,10 @@
         <v>101</v>
       </c>
       <c r="W47" s="1" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="48" spans="1:28" ht="145" x14ac:dyDescent="0.35">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="48" spans="1:28" ht="75" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -4026,28 +4027,28 @@
         <v>30</v>
       </c>
       <c r="C48" t="s">
+        <v>282</v>
+      </c>
+      <c r="D48" t="s">
+        <v>283</v>
+      </c>
+      <c r="E48" t="s">
+        <v>283</v>
+      </c>
+      <c r="F48" t="s">
+        <v>56</v>
+      </c>
+      <c r="I48" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="D48" t="s">
+      <c r="J48" t="s">
         <v>285</v>
       </c>
-      <c r="E48" t="s">
-        <v>285</v>
-      </c>
-      <c r="F48" t="s">
-        <v>56</v>
-      </c>
-      <c r="I48" s="1" t="s">
+      <c r="K48" t="s">
         <v>286</v>
       </c>
-      <c r="J48" t="s">
+      <c r="Q48" s="1" t="s">
         <v>287</v>
-      </c>
-      <c r="K48" t="s">
-        <v>288</v>
-      </c>
-      <c r="Q48" s="1" t="s">
-        <v>289</v>
       </c>
       <c r="T48" t="s">
         <v>36</v>
@@ -4059,10 +4060,10 @@
         <v>60</v>
       </c>
       <c r="W48" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="49" spans="1:28" ht="29" x14ac:dyDescent="0.35">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="49" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -4070,19 +4071,19 @@
         <v>30</v>
       </c>
       <c r="C49" t="s">
+        <v>289</v>
+      </c>
+      <c r="D49" t="s">
+        <v>290</v>
+      </c>
+      <c r="E49" t="s">
         <v>291</v>
       </c>
-      <c r="D49" t="s">
+      <c r="F49" t="s">
+        <v>56</v>
+      </c>
+      <c r="I49" s="1" t="s">
         <v>292</v>
-      </c>
-      <c r="E49" t="s">
-        <v>293</v>
-      </c>
-      <c r="F49" t="s">
-        <v>56</v>
-      </c>
-      <c r="I49" s="1" t="s">
-        <v>294</v>
       </c>
       <c r="J49" t="s">
         <v>47</v>
@@ -4100,7 +4101,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="50" spans="1:28" ht="29" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -4108,19 +4109,19 @@
         <v>30</v>
       </c>
       <c r="C50" t="s">
+        <v>293</v>
+      </c>
+      <c r="D50" t="s">
+        <v>294</v>
+      </c>
+      <c r="E50" t="s">
         <v>295</v>
       </c>
-      <c r="D50" t="s">
-        <v>296</v>
-      </c>
-      <c r="E50" t="s">
-        <v>297</v>
-      </c>
       <c r="F50" t="s">
         <v>56</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="J50" t="s">
         <v>47</v>
@@ -4138,7 +4139,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="51" spans="1:28" ht="29" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -4146,19 +4147,19 @@
         <v>30</v>
       </c>
       <c r="C51" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="D51" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E51" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="F51" t="s">
         <v>56</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="J51" t="s">
         <v>47</v>
@@ -4176,7 +4177,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="52" spans="1:28" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:28" ht="45" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -4184,19 +4185,19 @@
         <v>30</v>
       </c>
       <c r="C52" t="s">
+        <v>298</v>
+      </c>
+      <c r="D52" t="s">
+        <v>299</v>
+      </c>
+      <c r="E52" t="s">
+        <v>299</v>
+      </c>
+      <c r="F52" t="s">
+        <v>56</v>
+      </c>
+      <c r="I52" s="1" t="s">
         <v>300</v>
-      </c>
-      <c r="D52" t="s">
-        <v>301</v>
-      </c>
-      <c r="E52" t="s">
-        <v>301</v>
-      </c>
-      <c r="F52" t="s">
-        <v>56</v>
-      </c>
-      <c r="I52" s="1" t="s">
-        <v>302</v>
       </c>
       <c r="J52" t="s">
         <v>47</v>
@@ -4214,7 +4215,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="53" spans="1:28" ht="29" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -4222,19 +4223,19 @@
         <v>30</v>
       </c>
       <c r="C53" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D53" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="E53" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="F53" t="s">
         <v>56</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="J53" t="s">
         <v>47</v>
@@ -4252,7 +4253,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="54" spans="1:28" ht="29" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -4260,19 +4261,19 @@
         <v>30</v>
       </c>
       <c r="C54" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D54" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="E54" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="F54" t="s">
         <v>56</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="J54" t="s">
         <v>47</v>
@@ -4290,7 +4291,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="55" spans="1:28" ht="29" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -4298,19 +4299,19 @@
         <v>30</v>
       </c>
       <c r="C55" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D55" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="E55" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="F55" t="s">
         <v>56</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="J55" t="s">
         <v>47</v>
@@ -4328,7 +4329,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="56" spans="1:28" ht="29" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -4336,19 +4337,19 @@
         <v>30</v>
       </c>
       <c r="C56" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D56" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E56" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="F56" t="s">
         <v>56</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="J56" t="s">
         <v>47</v>
@@ -4366,13 +4367,13 @@
         <v>84</v>
       </c>
       <c r="AA56" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="AB56" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="57" spans="1:28" ht="29" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -4380,19 +4381,19 @@
         <v>30</v>
       </c>
       <c r="C57" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D57" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E57" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="F57" t="s">
         <v>56</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="J57" t="s">
         <v>47</v>
@@ -4410,7 +4411,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="58" spans="1:28" ht="29" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -4418,19 +4419,19 @@
         <v>30</v>
       </c>
       <c r="C58" t="s">
+        <v>312</v>
+      </c>
+      <c r="D58" t="s">
+        <v>313</v>
+      </c>
+      <c r="E58" t="s">
         <v>314</v>
       </c>
-      <c r="D58" t="s">
-        <v>315</v>
-      </c>
-      <c r="E58" t="s">
-        <v>316</v>
-      </c>
       <c r="F58" t="s">
         <v>56</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="J58" t="s">
         <v>47</v>
@@ -4448,7 +4449,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="59" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -4456,13 +4457,13 @@
         <v>30</v>
       </c>
       <c r="C59" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D59" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="E59" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="F59" t="s">
         <v>56</v>
@@ -4483,7 +4484,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="60" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -4491,13 +4492,13 @@
         <v>30</v>
       </c>
       <c r="C60" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D60" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="E60" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="F60" t="s">
         <v>56</v>
@@ -4518,7 +4519,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="61" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -4526,13 +4527,13 @@
         <v>30</v>
       </c>
       <c r="C61" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D61" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="E61" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="F61" t="s">
         <v>56</v>
@@ -4553,7 +4554,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="62" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
@@ -4561,13 +4562,13 @@
         <v>30</v>
       </c>
       <c r="C62" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D62" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="E62" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="F62" t="s">
         <v>56</v>
@@ -4588,7 +4589,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="63" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
@@ -4596,13 +4597,13 @@
         <v>30</v>
       </c>
       <c r="C63" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D63" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="E63" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="F63" t="s">
         <v>56</v>
@@ -4623,7 +4624,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="64" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
@@ -4631,13 +4632,13 @@
         <v>30</v>
       </c>
       <c r="C64" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D64" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="E64" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="F64" t="s">
         <v>56</v>
@@ -4658,7 +4659,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="65" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
@@ -4666,13 +4667,13 @@
         <v>30</v>
       </c>
       <c r="C65" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D65" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="E65" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="F65" t="s">
         <v>56</v>
@@ -4693,7 +4694,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="66" spans="1:24" ht="246.5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
@@ -4701,19 +4702,19 @@
         <v>30</v>
       </c>
       <c r="C66" t="s">
+        <v>329</v>
+      </c>
+      <c r="D66" t="s">
+        <v>330</v>
+      </c>
+      <c r="E66" t="s">
+        <v>330</v>
+      </c>
+      <c r="F66" t="s">
+        <v>56</v>
+      </c>
+      <c r="I66" s="1" t="s">
         <v>331</v>
-      </c>
-      <c r="D66" t="s">
-        <v>332</v>
-      </c>
-      <c r="E66" t="s">
-        <v>332</v>
-      </c>
-      <c r="F66" t="s">
-        <v>56</v>
-      </c>
-      <c r="I66" s="1" t="s">
-        <v>333</v>
       </c>
       <c r="J66" t="s">
         <v>47</v>
@@ -4731,7 +4732,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="67" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
@@ -4739,19 +4740,19 @@
         <v>30</v>
       </c>
       <c r="C67" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="D67" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="E67" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="F67" t="s">
         <v>106</v>
       </c>
       <c r="G67" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="J67" t="s">
         <v>47</v>
@@ -4769,7 +4770,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="68" spans="1:24" ht="275.5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:24" ht="135" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
@@ -4777,19 +4778,19 @@
         <v>30</v>
       </c>
       <c r="C68" t="s">
+        <v>335</v>
+      </c>
+      <c r="D68" t="s">
+        <v>336</v>
+      </c>
+      <c r="E68" t="s">
+        <v>336</v>
+      </c>
+      <c r="F68" t="s">
+        <v>56</v>
+      </c>
+      <c r="I68" s="1" t="s">
         <v>337</v>
-      </c>
-      <c r="D68" t="s">
-        <v>338</v>
-      </c>
-      <c r="E68" t="s">
-        <v>338</v>
-      </c>
-      <c r="F68" t="s">
-        <v>56</v>
-      </c>
-      <c r="I68" s="1" t="s">
-        <v>339</v>
       </c>
       <c r="J68" t="s">
         <v>47</v>
@@ -4807,7 +4808,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="69" spans="1:24" ht="87" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
@@ -4815,22 +4816,22 @@
         <v>30</v>
       </c>
       <c r="C69" t="s">
+        <v>338</v>
+      </c>
+      <c r="D69" t="s">
+        <v>339</v>
+      </c>
+      <c r="E69" t="s">
+        <v>339</v>
+      </c>
+      <c r="F69" t="s">
+        <v>56</v>
+      </c>
+      <c r="I69" s="1" t="s">
         <v>340</v>
       </c>
-      <c r="D69" t="s">
+      <c r="J69" t="s">
         <v>341</v>
-      </c>
-      <c r="E69" t="s">
-        <v>341</v>
-      </c>
-      <c r="F69" t="s">
-        <v>56</v>
-      </c>
-      <c r="I69" s="1" t="s">
-        <v>342</v>
-      </c>
-      <c r="J69" t="s">
-        <v>343</v>
       </c>
       <c r="T69" t="s">
         <v>36</v>
@@ -4845,10 +4846,10 @@
         <v>67</v>
       </c>
       <c r="X69" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="70" spans="1:24" ht="409.5" x14ac:dyDescent="0.35">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="70" spans="1:24" ht="150" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
@@ -4856,28 +4857,28 @@
         <v>30</v>
       </c>
       <c r="C70" t="s">
+        <v>343</v>
+      </c>
+      <c r="D70" t="s">
+        <v>344</v>
+      </c>
+      <c r="E70" t="s">
+        <v>344</v>
+      </c>
+      <c r="F70" t="s">
+        <v>56</v>
+      </c>
+      <c r="I70" s="1" t="s">
         <v>345</v>
       </c>
-      <c r="D70" t="s">
+      <c r="J70" s="1" t="s">
         <v>346</v>
       </c>
-      <c r="E70" t="s">
-        <v>346</v>
-      </c>
-      <c r="F70" t="s">
-        <v>56</v>
-      </c>
-      <c r="I70" s="1" t="s">
+      <c r="K70" t="s">
         <v>347</v>
       </c>
-      <c r="J70" s="1" t="s">
+      <c r="M70" s="1" t="s">
         <v>348</v>
-      </c>
-      <c r="K70" t="s">
-        <v>349</v>
-      </c>
-      <c r="M70" s="1" t="s">
-        <v>350</v>
       </c>
       <c r="T70" t="s">
         <v>36</v>
@@ -4889,10 +4890,10 @@
         <v>101</v>
       </c>
       <c r="W70" s="1" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="71" spans="1:24" ht="406" x14ac:dyDescent="0.35">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="71" spans="1:24" ht="90" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
@@ -4900,28 +4901,28 @@
         <v>30</v>
       </c>
       <c r="C71" t="s">
+        <v>349</v>
+      </c>
+      <c r="D71" t="s">
+        <v>350</v>
+      </c>
+      <c r="E71" t="s">
+        <v>350</v>
+      </c>
+      <c r="F71" t="s">
+        <v>56</v>
+      </c>
+      <c r="I71" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="J71" t="s">
         <v>351</v>
       </c>
-      <c r="D71" t="s">
+      <c r="K71" t="s">
+        <v>347</v>
+      </c>
+      <c r="M71" s="1" t="s">
         <v>352</v>
-      </c>
-      <c r="E71" t="s">
-        <v>352</v>
-      </c>
-      <c r="F71" t="s">
-        <v>56</v>
-      </c>
-      <c r="I71" s="1" t="s">
-        <v>347</v>
-      </c>
-      <c r="J71" t="s">
-        <v>353</v>
-      </c>
-      <c r="K71" t="s">
-        <v>349</v>
-      </c>
-      <c r="M71" s="1" t="s">
-        <v>354</v>
       </c>
       <c r="T71" t="s">
         <v>36</v>
@@ -4933,10 +4934,10 @@
         <v>101</v>
       </c>
       <c r="W71" s="1" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="72" spans="1:24" ht="406" x14ac:dyDescent="0.35">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="72" spans="1:24" ht="90" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
@@ -4944,28 +4945,28 @@
         <v>30</v>
       </c>
       <c r="C72" t="s">
+        <v>353</v>
+      </c>
+      <c r="D72" t="s">
+        <v>354</v>
+      </c>
+      <c r="E72" t="s">
+        <v>354</v>
+      </c>
+      <c r="F72" t="s">
+        <v>56</v>
+      </c>
+      <c r="I72" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="J72" t="s">
         <v>355</v>
       </c>
-      <c r="D72" t="s">
+      <c r="K72" t="s">
+        <v>347</v>
+      </c>
+      <c r="M72" s="1" t="s">
         <v>356</v>
-      </c>
-      <c r="E72" t="s">
-        <v>356</v>
-      </c>
-      <c r="F72" t="s">
-        <v>56</v>
-      </c>
-      <c r="I72" s="1" t="s">
-        <v>347</v>
-      </c>
-      <c r="J72" t="s">
-        <v>357</v>
-      </c>
-      <c r="K72" t="s">
-        <v>349</v>
-      </c>
-      <c r="M72" s="1" t="s">
-        <v>358</v>
       </c>
       <c r="T72" t="s">
         <v>36</v>
@@ -4977,10 +4978,10 @@
         <v>101</v>
       </c>
       <c r="W72" s="1" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="73" spans="1:24" ht="409.5" x14ac:dyDescent="0.35">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="73" spans="1:24" ht="165" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
@@ -4988,40 +4989,40 @@
         <v>30</v>
       </c>
       <c r="C73" t="s">
+        <v>357</v>
+      </c>
+      <c r="D73" t="s">
+        <v>358</v>
+      </c>
+      <c r="E73" t="s">
         <v>359</v>
       </c>
-      <c r="D73" t="s">
+      <c r="F73" t="s">
+        <v>56</v>
+      </c>
+      <c r="I73" s="1" t="s">
         <v>360</v>
       </c>
-      <c r="E73" t="s">
+      <c r="J73" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="F73" t="s">
-        <v>56</v>
-      </c>
-      <c r="I73" s="1" t="s">
+      <c r="T73" t="s">
+        <v>84</v>
+      </c>
+      <c r="U73" t="s">
         <v>362</v>
       </c>
-      <c r="J73" s="1" t="s">
+      <c r="V73" t="s">
+        <v>84</v>
+      </c>
+      <c r="W73" t="s">
+        <v>84</v>
+      </c>
+      <c r="X73" t="s">
         <v>363</v>
       </c>
-      <c r="T73" t="s">
-        <v>84</v>
-      </c>
-      <c r="U73" t="s">
-        <v>364</v>
-      </c>
-      <c r="V73" t="s">
-        <v>84</v>
-      </c>
-      <c r="W73" t="s">
-        <v>84</v>
-      </c>
-      <c r="X73" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="74" spans="1:24" ht="409.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="74" spans="1:24" ht="195" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
@@ -5029,28 +5030,28 @@
         <v>30</v>
       </c>
       <c r="C74" t="s">
+        <v>364</v>
+      </c>
+      <c r="D74" t="s">
+        <v>365</v>
+      </c>
+      <c r="E74" t="s">
         <v>366</v>
       </c>
-      <c r="D74" t="s">
+      <c r="F74" t="s">
+        <v>56</v>
+      </c>
+      <c r="I74" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="E74" t="s">
+      <c r="J74" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="K74" t="s">
         <v>368</v>
       </c>
-      <c r="F74" t="s">
-        <v>56</v>
-      </c>
-      <c r="I74" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="J74" s="1" t="s">
-        <v>363</v>
-      </c>
-      <c r="K74" t="s">
-        <v>370</v>
-      </c>
       <c r="M74" s="1" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="T74" t="s">
         <v>36</v>
@@ -5062,10 +5063,10 @@
         <v>101</v>
       </c>
       <c r="W74" s="1" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="75" spans="1:24" ht="409.5" x14ac:dyDescent="0.35">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="75" spans="1:24" ht="180" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
@@ -5073,28 +5074,28 @@
         <v>30</v>
       </c>
       <c r="C75" t="s">
+        <v>369</v>
+      </c>
+      <c r="D75" t="s">
+        <v>370</v>
+      </c>
+      <c r="E75" t="s">
         <v>371</v>
       </c>
-      <c r="D75" t="s">
+      <c r="F75" t="s">
+        <v>56</v>
+      </c>
+      <c r="I75" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="E75" t="s">
+      <c r="J75" s="1" t="s">
         <v>373</v>
       </c>
-      <c r="F75" t="s">
-        <v>56</v>
-      </c>
-      <c r="I75" s="1" t="s">
+      <c r="K75" t="s">
         <v>374</v>
       </c>
-      <c r="J75" s="1" t="s">
-        <v>375</v>
-      </c>
-      <c r="K75" t="s">
-        <v>376</v>
-      </c>
       <c r="M75" s="1" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="T75" t="s">
         <v>36</v>
@@ -5106,10 +5107,10 @@
         <v>101</v>
       </c>
       <c r="W75" s="1" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="76" spans="1:24" ht="409.5" x14ac:dyDescent="0.35">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="76" spans="1:24" ht="135" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
@@ -5117,28 +5118,28 @@
         <v>30</v>
       </c>
       <c r="C76" t="s">
+        <v>375</v>
+      </c>
+      <c r="D76" t="s">
+        <v>376</v>
+      </c>
+      <c r="E76" t="s">
         <v>377</v>
       </c>
-      <c r="D76" t="s">
+      <c r="F76" t="s">
+        <v>56</v>
+      </c>
+      <c r="G76" t="s">
+        <v>334</v>
+      </c>
+      <c r="J76" t="s">
         <v>378</v>
       </c>
-      <c r="E76" t="s">
+      <c r="K76" s="1" t="s">
         <v>379</v>
       </c>
-      <c r="F76" t="s">
-        <v>56</v>
-      </c>
-      <c r="G76" t="s">
-        <v>336</v>
-      </c>
-      <c r="J76" t="s">
+      <c r="Q76" t="s">
         <v>380</v>
-      </c>
-      <c r="K76" s="1" t="s">
-        <v>381</v>
-      </c>
-      <c r="Q76" t="s">
-        <v>382</v>
       </c>
       <c r="T76" t="s">
         <v>36</v>
@@ -5147,16 +5148,16 @@
         <v>74</v>
       </c>
       <c r="V76" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="W76" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="X76" s="1" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="77" spans="1:24" ht="409.5" x14ac:dyDescent="0.35">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="77" spans="1:24" ht="165" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
@@ -5164,28 +5165,28 @@
         <v>30</v>
       </c>
       <c r="C77" t="s">
+        <v>382</v>
+      </c>
+      <c r="D77" t="s">
+        <v>383</v>
+      </c>
+      <c r="E77" t="s">
         <v>384</v>
       </c>
-      <c r="D77" t="s">
+      <c r="F77" t="s">
+        <v>56</v>
+      </c>
+      <c r="I77" s="1" t="s">
         <v>385</v>
       </c>
-      <c r="E77" t="s">
+      <c r="J77" t="s">
+        <v>378</v>
+      </c>
+      <c r="K77" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="F77" t="s">
-        <v>56</v>
-      </c>
-      <c r="I77" s="1" t="s">
-        <v>387</v>
-      </c>
-      <c r="J77" t="s">
+      <c r="Q77" t="s">
         <v>380</v>
-      </c>
-      <c r="K77" s="1" t="s">
-        <v>388</v>
-      </c>
-      <c r="Q77" t="s">
-        <v>382</v>
       </c>
       <c r="T77" t="s">
         <v>36</v>
@@ -5197,10 +5198,10 @@
         <v>101</v>
       </c>
       <c r="W77" s="1" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="78" spans="1:24" ht="159.5" x14ac:dyDescent="0.35">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="78" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>77</v>
       </c>
@@ -5208,19 +5209,19 @@
         <v>30</v>
       </c>
       <c r="C78" t="s">
+        <v>387</v>
+      </c>
+      <c r="D78" t="s">
+        <v>388</v>
+      </c>
+      <c r="E78" t="s">
         <v>389</v>
       </c>
-      <c r="D78" t="s">
+      <c r="F78" t="s">
+        <v>56</v>
+      </c>
+      <c r="I78" s="1" t="s">
         <v>390</v>
-      </c>
-      <c r="E78" t="s">
-        <v>391</v>
-      </c>
-      <c r="F78" t="s">
-        <v>56</v>
-      </c>
-      <c r="I78" s="1" t="s">
-        <v>392</v>
       </c>
       <c r="J78" t="s">
         <v>47</v>
@@ -5238,7 +5239,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="79" spans="1:24" ht="333.5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
@@ -5246,19 +5247,19 @@
         <v>30</v>
       </c>
       <c r="C79" t="s">
+        <v>391</v>
+      </c>
+      <c r="D79" t="s">
+        <v>392</v>
+      </c>
+      <c r="E79" t="s">
+        <v>392</v>
+      </c>
+      <c r="F79" t="s">
+        <v>56</v>
+      </c>
+      <c r="I79" s="1" t="s">
         <v>393</v>
-      </c>
-      <c r="D79" t="s">
-        <v>394</v>
-      </c>
-      <c r="E79" t="s">
-        <v>394</v>
-      </c>
-      <c r="F79" t="s">
-        <v>56</v>
-      </c>
-      <c r="I79" s="1" t="s">
-        <v>395</v>
       </c>
       <c r="J79" t="s">
         <v>47</v>
@@ -5276,7 +5277,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="80" spans="1:24" ht="29" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>79</v>
       </c>
@@ -5284,19 +5285,19 @@
         <v>30</v>
       </c>
       <c r="C80" t="s">
+        <v>394</v>
+      </c>
+      <c r="D80" t="s">
+        <v>395</v>
+      </c>
+      <c r="E80" t="s">
         <v>396</v>
       </c>
-      <c r="D80" t="s">
-        <v>397</v>
-      </c>
-      <c r="E80" t="s">
-        <v>398</v>
-      </c>
       <c r="F80" t="s">
         <v>56</v>
       </c>
       <c r="I80" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="J80" t="s">
         <v>47</v>
@@ -5314,7 +5315,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="81" spans="1:23" ht="29" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>80</v>
       </c>
@@ -5322,19 +5323,19 @@
         <v>30</v>
       </c>
       <c r="C81" t="s">
+        <v>397</v>
+      </c>
+      <c r="D81" t="s">
+        <v>398</v>
+      </c>
+      <c r="E81" t="s">
         <v>399</v>
       </c>
-      <c r="D81" t="s">
-        <v>400</v>
-      </c>
-      <c r="E81" t="s">
-        <v>401</v>
-      </c>
       <c r="F81" t="s">
         <v>56</v>
       </c>
       <c r="I81" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="J81" t="s">
         <v>47</v>
@@ -5352,7 +5353,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="82" spans="1:23" ht="29" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>81</v>
       </c>
@@ -5360,19 +5361,19 @@
         <v>30</v>
       </c>
       <c r="C82" t="s">
+        <v>400</v>
+      </c>
+      <c r="D82" t="s">
+        <v>401</v>
+      </c>
+      <c r="E82" t="s">
         <v>402</v>
       </c>
-      <c r="D82" t="s">
-        <v>403</v>
-      </c>
-      <c r="E82" t="s">
-        <v>404</v>
-      </c>
       <c r="F82" t="s">
         <v>56</v>
       </c>
       <c r="I82" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="J82" t="s">
         <v>47</v>
@@ -5390,7 +5391,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="83" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>82</v>
       </c>
@@ -5398,13 +5399,13 @@
         <v>30</v>
       </c>
       <c r="C83" t="s">
+        <v>403</v>
+      </c>
+      <c r="D83" t="s">
+        <v>404</v>
+      </c>
+      <c r="E83" t="s">
         <v>405</v>
-      </c>
-      <c r="D83" t="s">
-        <v>406</v>
-      </c>
-      <c r="E83" t="s">
-        <v>407</v>
       </c>
       <c r="F83" t="s">
         <v>56</v>
@@ -5425,7 +5426,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="84" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>83</v>
       </c>
@@ -5433,19 +5434,19 @@
         <v>30</v>
       </c>
       <c r="C84" t="s">
+        <v>406</v>
+      </c>
+      <c r="D84" t="s">
+        <v>407</v>
+      </c>
+      <c r="E84" t="s">
         <v>408</v>
       </c>
-      <c r="D84" t="s">
+      <c r="F84" t="s">
+        <v>56</v>
+      </c>
+      <c r="G84" t="s">
         <v>409</v>
-      </c>
-      <c r="E84" t="s">
-        <v>410</v>
-      </c>
-      <c r="F84" t="s">
-        <v>56</v>
-      </c>
-      <c r="G84" t="s">
-        <v>411</v>
       </c>
       <c r="J84" t="s">
         <v>47</v>

</xml_diff>

<commit_message>
Add harmo rle for missing variables
date: Response is date with yyyy-mm-dd.
period_fasted: Response options are: 12 hours or longer, between 8 and 12 hours, less than 8 hours, and
unknown (character)
 
WRKA13_total_working_hours: Response in hours
 
WRKC02_occupation_category: Response are numeric and range between 0 to 14.
 
TOXB_area: Response are numeric and range between 1 to 2.
FND00_currently_smoke: !! This question was not asked at baseline, only during follow-up.
</commit_message>
<xml_diff>
--- a/data_processing_elements-HBS.xlsx
+++ b/data_processing_elements-HBS.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/849507f40a0f895e/Documents/ProPASS/Studies/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21FECD06-E538-448D-9825-ABEB02DADF4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{09B0DEE3-935C-46B5-B8C0-152FC6679B3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{A2851C76-6816-460F-844D-5B34B01F8802}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{AA860D54-F729-477E-8EFC-6CB92CB671B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1032" uniqueCount="421">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1025" uniqueCount="416">
   <si>
     <t>index</t>
   </si>
@@ -179,10 +179,7 @@
     <t>yyyy-mm-dd</t>
   </si>
   <si>
-    <t>__BLANK__</t>
-  </si>
-  <si>
-    <t>undetermined</t>
+    <t>direct_mapping</t>
   </si>
   <si>
     <t>There is 3 lab visit, we are taking the first one (need the date)</t>
@@ -240,9 +237,6 @@
   <si>
     <t>Value: Age in years, specified as the age of the participant at the time of the first visit to the lab. 
 Calculated as the time between the participant’s date of birth, and the date they completed their first lab visit.</t>
-  </si>
-  <si>
-    <t>direct_mapping</t>
   </si>
   <si>
     <t>sdc_education</t>
@@ -258,6 +252,9 @@
 1 = High school qualifications ; 
 2 = Further education qualifications ; 
 3 = University degree and higher</t>
+  </si>
+  <si>
+    <t>LIS07_education_completed</t>
   </si>
   <si>
     <t>What is the highest level of education that you have completed with diploma or certificate?</t>
@@ -325,6 +322,9 @@
 2 = Black or African American (Eg: African American, Jamaican, Haitian, Nigerian, Ethiopian, Somalian, etc) ; 
 3 = Asian (Eg: Chinese, Filipino, Asian Indian, Vietnamese, Korean, Japanese, etc) ; 
 4 = Mixed ethnicity and Other</t>
+  </si>
+  <si>
+    <t>__BLANK__</t>
   </si>
   <si>
     <t>impossible</t>
@@ -477,6 +477,12 @@
 1 = Retired</t>
   </si>
   <si>
+    <t>case_when(
+LIS05b_situations_pursuits_most == 9 ~ 1L;
+LIS05b_situations_pursuits_most %in% c(1:8,10:14) ~ 0L;
+ELSE ~ NA)</t>
+  </si>
+  <si>
     <t>participants are between 30-39 so there should not be any retired person</t>
   </si>
   <si>
@@ -666,6 +672,11 @@
     <t>Method used to measure the body fat percentage</t>
   </si>
   <si>
+    <t>case_when(
+!is.na(BOD109_fat_percentage) ~ "Bioelectrical impedance measurement (Bodystat Multi-Scan 5000)";
+ELSE ~ NA_character_)</t>
+  </si>
+  <si>
     <t>pm_systo_bp</t>
   </si>
   <si>
@@ -736,6 +747,9 @@
     <t>ml/min/kg</t>
   </si>
   <si>
+    <t>rel..vo2max</t>
+  </si>
+  <si>
     <t>Refers to the relative vo2max calculated with the following formula: (abs. vo2max / weight) *1000</t>
   </si>
   <si>
@@ -754,6 +768,9 @@
   </si>
   <si>
     <t>period_fasted</t>
+  </si>
+  <si>
+    <t>incompatible</t>
   </si>
   <si>
     <t>lab_red_blood_cell_count</t>
@@ -966,30 +983,6 @@
     <t>0 = Never smoked ; 
 1 = Previously smoked ; 
 2 = Currently smoke</t>
-  </si>
-  <si>
-    <t>SMH04_ever_smoked;
-FND00_currently_smoke</t>
-  </si>
-  <si>
-    <t>Have you ever smoked?;
-Do you currently smoke?</t>
-  </si>
-  <si>
-    <t>0 = no
-1 = a few times to try
-2 = yes
-0 = no 
-1 = yes 
-2 = yes, I have started after the previous labvisit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">case_when(
-SMH04_ever_smoked == 2 &amp; FND00_currently_smoke %in% c(1, 2) ~ 2L;
-SMH04_ever_smoked == 2 &amp; FND00_currently_smoke == 0 ~ 1L;
-SMH04_ever_smoked %in% c(0, 1) ~ 0L;
-ELSE ~ NA_integer_)
-</t>
   </si>
   <si>
     <t>smk_smoking_frequency</t>
@@ -1277,6 +1270,13 @@
 bed) doing the following?</t>
   </si>
   <si>
+    <t>case_when(
+(as.numeric(SBQ12_watch_television_wd)*5 + as.numeric(SBQ22_watch_television_we)*2)/7 &lt;= 1 ~ 1L; 
+(as.numeric(SBQ12_watch_television_wd)*5 + as.numeric(SBQ22_watch_television_we)*2)/7 &gt; 1 &amp; (as.numeric(SBQ12_watch_television_wd)*5 + as.numeric(SBQ22_watch_television_we)*2)/7 &lt;= 3 ~ 2L;
+(as.numeric(SBQ12_watch_television_wd)*5 + as.numeric(SBQ22_watch_television_we)*2)/7 &gt; 3 ~ 3L;
+ELSE ~ NA_integer_)</t>
+  </si>
+  <si>
     <t>sed_beh_tv_week_days</t>
   </si>
   <si>
@@ -1290,6 +1290,13 @@
 doing the following?</t>
   </si>
   <si>
+    <t>case_when(
+as.numeric(SBQ12_watch_television_wd) &lt;= 1 ~ 1L; 
+as.numeric(SBQ12_watch_television_wd) &gt; 1 &amp; as.numeric(SBQ12_watch_television_wd) &lt;= 3 ~ 2L;
+as.numeric(SBQ12_watch_television_wd) &gt; 3 ~ 3L;
+ELSE ~ NA_integer_)</t>
+  </si>
+  <si>
     <t>sed_beh_tv_weekend_days</t>
   </si>
   <si>
@@ -1301,6 +1308,13 @@
   <si>
     <t>On a typical WEEKENDDAY, how much time do you spend (from when you wake up until you go to 
 bed) doing the following?</t>
+  </si>
+  <si>
+    <t>case_when(
+as.numeric(SBQ22_watch_television_we)&lt;= 1 ~ 1L; 
+as.numeric(SBQ22_watch_television_we)&gt; 1 &amp; as.numeric(SBQ22_watch_television_we)&lt;= 3 ~ 2L;
+as.numeric(SBQ22_watch_television_we)&gt; 3 ~ 3L;
+ELSE ~ NA_integer_)</t>
   </si>
   <si>
     <t>sed_beh_comp_use</t>
@@ -1329,9 +1343,6 @@
 SBQ24_computer_outside_office_we</t>
   </si>
   <si>
-    <t>incompatible</t>
-  </si>
-  <si>
     <t>we have "Playing computer or video games, using a tablet (outside of work)" but includes playing video games on a console and tablet</t>
   </si>
   <si>
@@ -1352,6 +1363,13 @@
     <t>Playing computer or video games, using a tablet (outside of work)</t>
   </si>
   <si>
+    <t>case_when(
+(as.numeric(SBQ14_computer_outside_office_wd)*5 + as.numeric(SBQ24_computer_outside_office_we)*2)/7 &lt;= 1 ~ 1L; 
+(as.numeric(SBQ14_computer_outside_office_wd)*5 + as.numeric(SBQ24_computer_outside_office_we)*2)/7 &gt; 1 &amp; (as.numeric(SBQ14_computer_outside_office_wd)*5 + as.numeric(SBQ24_computer_outside_office_we)*2)/7 &lt;= 3 ~ 2L;
+(as.numeric(SBQ14_computer_outside_office_wd)*5 + as.numeric(SBQ24_computer_outside_office_we)*2)/7 &gt; 3 ~ 3L;
+ELSE ~ NA_integer_)</t>
+  </si>
+  <si>
     <t>sed_beh_reading</t>
   </si>
   <si>
@@ -1373,6 +1391,13 @@
     <t>Sitting reading a book or magazine</t>
   </si>
   <si>
+    <t>case_when(
+(as.numeric(SBQ18_read_book_magazine_wd)*5 + as.numeric(SBQ28_read_book_magazine_we)*2)/7 &lt;= 1 ~ 1L; 
+(as.numeric(SBQ18_read_book_magazine_wd)*5 + as.numeric(SBQ28_read_book_magazine_we)*2)/7 &gt; 1 &amp; (as.numeric(SBQ18_read_book_magazine_wd)*5 + as.numeric(SBQ28_read_book_magazine_we)*2)/7 &lt;= 3 ~ 2L;
+(as.numeric(SBQ18_read_book_magazine_wd)*5 + as.numeric(SBQ28_read_book_magazine_we)*2)/7 &gt; 3 ~ 3L;
+ELSE ~ NA_integer_)</t>
+  </si>
+  <si>
     <t>sed_beh_total_sitting</t>
   </si>
   <si>
@@ -1390,6 +1415,9 @@
   </si>
   <si>
     <t>Calculation: SBQ_total_week + SBQ_total_weekend</t>
+  </si>
+  <si>
+    <t>as.integer(as.numeric(SBQ_total)/7)</t>
   </si>
   <si>
     <t>Note from cohort: Please note that unlikely high values are present in the data, suggesting that those 
@@ -1418,121 +1446,6 @@
   <si>
     <t>Sumscore indicating the total time in hours spent on the activities during a full 7-
 day week</t>
-  </si>
-  <si>
-    <t>phy_walking</t>
-  </si>
-  <si>
-    <t>Walking for leisure</t>
-  </si>
-  <si>
-    <t>Frequency of walking for leisure per week</t>
-  </si>
-  <si>
-    <t>1 = Less than once a week ; 
-2 = 1 to 5 times a week ; 
-3 = 6 times or more a week</t>
-  </si>
-  <si>
-    <t>phy_occupational_pa</t>
-  </si>
-  <si>
-    <t>Occupational physical activity</t>
-  </si>
-  <si>
-    <t>1 = Mostly sedentary-no physical demands ; 
-2 = Mostly standing or walking ; 
-3 = Standing and walking with lifting or carrying ; 
-4 = Strenuous physical work</t>
-  </si>
-  <si>
-    <t>phy_sport_participation</t>
-  </si>
-  <si>
-    <t>Sport participation</t>
-  </si>
-  <si>
-    <t>Indicator of whether the participant is participating in sport activity or not</t>
-  </si>
-  <si>
-    <t>phy_active_commuting</t>
-  </si>
-  <si>
-    <t>Active commuting</t>
-  </si>
-  <si>
-    <t>Indicator of whether the participant is engaging in active commuting</t>
-  </si>
-  <si>
-    <t>phy_leisure_time</t>
-  </si>
-  <si>
-    <t>Leisure-time physical activity, including sport</t>
-  </si>
-  <si>
-    <t>Indicator of whether the participant is engaging in physical activity during leisure-time (including sport)</t>
-  </si>
-  <si>
-    <t>phy_mobility_limitation_SF36</t>
-  </si>
-  <si>
-    <t>Physical function SF36 subscale score</t>
-  </si>
-  <si>
-    <t>Total score of the physical function subscale of SF38</t>
-  </si>
-  <si>
-    <t>phy_SF36_nb_items</t>
-  </si>
-  <si>
-    <t>Number of non-missing items</t>
-  </si>
-  <si>
-    <t>Number of non-missing items in the SF36 physical function subscale</t>
-  </si>
-  <si>
-    <t>items</t>
-  </si>
-  <si>
-    <t>LIS07_education_completed</t>
-  </si>
-  <si>
-    <t>rel..vo2max</t>
-  </si>
-  <si>
-    <t>case_when(
-(as.numeric(SBQ12_watch_television_wd)*5 + as.numeric(SBQ22_watch_television_we)*2)/7 &lt;= 1 ~ 1L; 
-(as.numeric(SBQ12_watch_television_wd)*5 + as.numeric(SBQ22_watch_television_we)*2)/7 &gt; 1 &amp; (as.numeric(SBQ12_watch_television_wd)*5 + as.numeric(SBQ22_watch_television_we)*2)/7 &lt;= 3 ~ 2L;
-(as.numeric(SBQ12_watch_television_wd)*5 + as.numeric(SBQ22_watch_television_we)*2)/7 &gt; 3 ~ 3L;
-ELSE ~ NA_integer_)</t>
-  </si>
-  <si>
-    <t>case_when(
-as.numeric(SBQ12_watch_television_wd) &lt;= 1 ~ 1L; 
-as.numeric(SBQ12_watch_television_wd) &gt; 1 &amp; as.numeric(SBQ12_watch_television_wd) &lt;= 3 ~ 2L;
-as.numeric(SBQ12_watch_television_wd) &gt; 3 ~ 3L;
-ELSE ~ NA_integer_)</t>
-  </si>
-  <si>
-    <t>case_when(
-as.numeric(SBQ22_watch_television_we)&lt;= 1 ~ 1L; 
-as.numeric(SBQ22_watch_television_we)&gt; 1 &amp; as.numeric(SBQ22_watch_television_we)&lt;= 3 ~ 2L;
-as.numeric(SBQ22_watch_television_we)&gt; 3 ~ 3L;
-ELSE ~ NA_integer_)</t>
-  </si>
-  <si>
-    <t>case_when(
-(as.numeric(SBQ14_computer_outside_office_wd)*5 + as.numeric(SBQ24_computer_outside_office_we)*2)/7 &lt;= 1 ~ 1L; 
-(as.numeric(SBQ14_computer_outside_office_wd)*5 + as.numeric(SBQ24_computer_outside_office_we)*2)/7 &gt; 1 &amp; (as.numeric(SBQ14_computer_outside_office_wd)*5 + as.numeric(SBQ24_computer_outside_office_we)*2)/7 &lt;= 3 ~ 2L;
-(as.numeric(SBQ14_computer_outside_office_wd)*5 + as.numeric(SBQ24_computer_outside_office_we)*2)/7 &gt; 3 ~ 3L;
-ELSE ~ NA_integer_)</t>
-  </si>
-  <si>
-    <t>case_when(
-(as.numeric(SBQ18_read_book_magazine_wd)*5 + as.numeric(SBQ28_read_book_magazine_we)*2)/7 &lt;= 1 ~ 1L; 
-(as.numeric(SBQ18_read_book_magazine_wd)*5 + as.numeric(SBQ28_read_book_magazine_we)*2)/7 &gt; 1 &amp; (as.numeric(SBQ18_read_book_magazine_wd)*5 + as.numeric(SBQ28_read_book_magazine_we)*2)/7 &lt;= 3 ~ 2L;
-(as.numeric(SBQ18_read_book_magazine_wd)*5 + as.numeric(SBQ28_read_book_magazine_we)*2)/7 &gt; 3 ~ 3L;
-ELSE ~ NA_integer_)</t>
   </si>
   <si>
     <t>case_when(
@@ -1545,18 +1458,78 @@
 ELSE ~ NA_integer_)</t>
   </si>
   <si>
-    <t>as.integer(as.numeric(SBQ_total)/7)</t>
-  </si>
-  <si>
-    <t>case_when(
-!is.na(BOD109_fat_percentage) ~ "Bioelectrical impedance measurement (Bodystat Multi-Scan 5000)";
-ELSE ~ NA_character_)</t>
-  </si>
-  <si>
-    <t>case_when(
-LIS05b_situations_pursuits_most == 9 ~ 1L;
-LIS05b_situations_pursuits_most %in% c(1:8,10:14) ~ 0L;
-ELSE ~ NA)</t>
+    <t>phy_walking</t>
+  </si>
+  <si>
+    <t>Walking for leisure</t>
+  </si>
+  <si>
+    <t>Frequency of walking for leisure per week</t>
+  </si>
+  <si>
+    <t>1 = Less than once a week ; 
+2 = 1 to 5 times a week ; 
+3 = 6 times or more a week</t>
+  </si>
+  <si>
+    <t>phy_occupational_pa</t>
+  </si>
+  <si>
+    <t>Occupational physical activity</t>
+  </si>
+  <si>
+    <t>1 = Mostly sedentary-no physical demands ; 
+2 = Mostly standing or walking ; 
+3 = Standing and walking with lifting or carrying ; 
+4 = Strenuous physical work</t>
+  </si>
+  <si>
+    <t>phy_sport_participation</t>
+  </si>
+  <si>
+    <t>Sport participation</t>
+  </si>
+  <si>
+    <t>Indicator of whether the participant is participating in sport activity or not</t>
+  </si>
+  <si>
+    <t>phy_active_commuting</t>
+  </si>
+  <si>
+    <t>Active commuting</t>
+  </si>
+  <si>
+    <t>Indicator of whether the participant is engaging in active commuting</t>
+  </si>
+  <si>
+    <t>phy_leisure_time</t>
+  </si>
+  <si>
+    <t>Leisure-time physical activity, including sport</t>
+  </si>
+  <si>
+    <t>Indicator of whether the participant is engaging in physical activity during leisure-time (including sport)</t>
+  </si>
+  <si>
+    <t>phy_mobility_limitation_SF36</t>
+  </si>
+  <si>
+    <t>Physical function SF36 subscale score</t>
+  </si>
+  <si>
+    <t>Total score of the physical function subscale of SF38</t>
+  </si>
+  <si>
+    <t>phy_SF36_nb_items</t>
+  </si>
+  <si>
+    <t>Number of non-missing items</t>
+  </si>
+  <si>
+    <t>Number of non-missing items in the SF36 physical function subscale</t>
+  </si>
+  <si>
+    <t>items</t>
   </si>
 </sst>
 </file>
@@ -1624,7 +1597,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1939,14 +1912,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1AF92DA-191C-4FF7-9A4B-8BE07EA34827}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5FD0B37-B6E8-454F-93F7-57FF9B64A4BB}">
   <dimension ref="A1:AD84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S13" workbookViewId="0">
-      <selection activeCell="W27" sqref="W27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="54.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="9" max="9" width="42.42578125" customWidth="1"/>
+    <col min="13" max="13" width="54" customWidth="1"/>
+    <col min="17" max="17" width="41.42578125" customWidth="1"/>
+    <col min="19" max="19" width="33.5703125" customWidth="1"/>
+    <col min="20" max="20" width="12" customWidth="1"/>
+    <col min="21" max="21" width="13.7109375" customWidth="1"/>
+    <col min="22" max="22" width="16.85546875" customWidth="1"/>
+    <col min="23" max="23" width="50" customWidth="1"/>
+    <col min="27" max="27" width="46.42578125" customWidth="1"/>
+    <col min="29" max="29" width="43.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
@@ -2107,31 +2092,31 @@
         <v>46</v>
       </c>
       <c r="J3" t="s">
+        <v>45</v>
+      </c>
+      <c r="T3" t="s">
+        <v>36</v>
+      </c>
+      <c r="U3" t="s">
+        <v>37</v>
+      </c>
+      <c r="V3" t="s">
         <v>47</v>
       </c>
-      <c r="T3" t="s">
+      <c r="W3" t="s">
+        <v>47</v>
+      </c>
+      <c r="X3" t="s">
         <v>48</v>
       </c>
-      <c r="U3" t="s">
-        <v>48</v>
-      </c>
-      <c r="V3" t="s">
-        <v>48</v>
-      </c>
-      <c r="W3" t="s">
-        <v>48</v>
-      </c>
-      <c r="X3" t="s">
+      <c r="AA3" t="s">
         <v>49</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="AB3" t="s">
         <v>50</v>
       </c>
-      <c r="AB3" t="s">
+      <c r="AC3" t="s">
         <v>51</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>52</v>
       </c>
       <c r="AD3" t="s">
         <v>41</v>
@@ -2145,28 +2130,28 @@
         <v>30</v>
       </c>
       <c r="C4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" t="s">
         <v>53</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>54</v>
       </c>
-      <c r="E4" t="s">
-        <v>55</v>
-      </c>
       <c r="F4" t="s">
+        <v>55</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="J4" t="s">
+        <v>53</v>
+      </c>
+      <c r="K4" t="s">
         <v>57</v>
       </c>
-      <c r="J4" t="s">
-        <v>54</v>
-      </c>
-      <c r="K4" t="s">
+      <c r="Q4" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="Q4" s="1" t="s">
-        <v>59</v>
       </c>
       <c r="T4" t="s">
         <v>36</v>
@@ -2175,10 +2160,10 @@
         <v>37</v>
       </c>
       <c r="V4" t="s">
+        <v>59</v>
+      </c>
+      <c r="W4" t="s">
         <v>60</v>
-      </c>
-      <c r="W4" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:30" ht="60" x14ac:dyDescent="0.25">
@@ -2189,25 +2174,25 @@
         <v>30</v>
       </c>
       <c r="C5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" t="s">
         <v>62</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>63</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
+        <v>55</v>
+      </c>
+      <c r="G5" t="s">
         <v>64</v>
       </c>
-      <c r="F5" t="s">
-        <v>56</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="J5" t="s">
+        <v>62</v>
+      </c>
+      <c r="M5" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="J5" t="s">
-        <v>63</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="T5" t="s">
         <v>36</v>
@@ -2216,10 +2201,10 @@
         <v>37</v>
       </c>
       <c r="V5" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="W5" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:30" ht="180" x14ac:dyDescent="0.25">
@@ -2230,58 +2215,58 @@
         <v>30</v>
       </c>
       <c r="C6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E6" t="s">
         <v>68</v>
       </c>
-      <c r="D6" t="s">
+      <c r="F6" t="s">
+        <v>55</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E6" t="s">
+      <c r="J6" t="s">
         <v>70</v>
       </c>
-      <c r="F6" t="s">
-        <v>56</v>
-      </c>
-      <c r="I6" s="1" t="s">
+      <c r="M6" t="s">
         <v>71</v>
       </c>
-      <c r="J6" t="s">
-        <v>410</v>
-      </c>
-      <c r="M6" t="s">
+      <c r="Q6" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="Q6" s="1" t="s">
-        <v>73</v>
       </c>
       <c r="T6" t="s">
         <v>36</v>
       </c>
       <c r="U6" t="s">
+        <v>73</v>
+      </c>
+      <c r="V6" t="s">
+        <v>59</v>
+      </c>
+      <c r="W6" t="s">
         <v>74</v>
       </c>
-      <c r="V6" t="s">
-        <v>60</v>
-      </c>
-      <c r="W6" t="s">
+      <c r="X6" t="s">
         <v>75</v>
       </c>
-      <c r="X6" t="s">
+      <c r="AA6" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="AA6" s="1" t="s">
+      <c r="AB6" t="s">
         <v>77</v>
       </c>
-      <c r="AB6" t="s">
+      <c r="AC6" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="AC6" s="1" t="s">
-        <v>79</v>
       </c>
       <c r="AD6" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:30" ht="105" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" ht="120" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2289,22 +2274,22 @@
         <v>30</v>
       </c>
       <c r="C7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D7" t="s">
         <v>80</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>81</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
+        <v>55</v>
+      </c>
+      <c r="I7" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="F7" t="s">
-        <v>56</v>
-      </c>
-      <c r="I7" s="1" t="s">
+      <c r="J7" t="s">
         <v>83</v>
-      </c>
-      <c r="J7" t="s">
-        <v>47</v>
       </c>
       <c r="T7" t="s">
         <v>84</v>
@@ -2322,7 +2307,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:30" ht="240" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30" ht="270" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2339,7 +2324,7 @@
         <v>89</v>
       </c>
       <c r="F8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>90</v>
@@ -2357,10 +2342,10 @@
         <v>36</v>
       </c>
       <c r="U8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="V8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="W8" t="s">
         <v>94</v>
@@ -2383,7 +2368,7 @@
         <v>97</v>
       </c>
       <c r="F9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>98</v>
@@ -2395,18 +2380,15 @@
         <v>100</v>
       </c>
       <c r="T9" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="U9" t="s">
-        <v>48</v>
+        <v>73</v>
       </c>
       <c r="V9" t="s">
-        <v>48</v>
+        <v>101</v>
       </c>
       <c r="W9" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="X9" s="1" t="s">
         <v>102</v>
       </c>
     </row>
@@ -2436,22 +2418,19 @@
         <v>100</v>
       </c>
       <c r="T10" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="U10" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="V10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="W10" t="s">
-        <v>48</v>
-      </c>
-      <c r="X10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="11" spans="1:30" ht="390" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2480,22 +2459,19 @@
         <v>112</v>
       </c>
       <c r="T11" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="U11" t="s">
-        <v>48</v>
+        <v>73</v>
       </c>
       <c r="V11" t="s">
-        <v>48</v>
+        <v>101</v>
       </c>
       <c r="W11" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="X11" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="12" spans="1:30" ht="240" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30" ht="270" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2512,7 +2488,7 @@
         <v>116</v>
       </c>
       <c r="F12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>117</v>
@@ -2530,16 +2506,16 @@
         <v>36</v>
       </c>
       <c r="U12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="V12" t="s">
         <v>101</v>
       </c>
       <c r="W12" s="1" t="s">
-        <v>420</v>
+        <v>118</v>
       </c>
       <c r="X12" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:30" ht="75" x14ac:dyDescent="0.25">
@@ -2550,40 +2526,40 @@
         <v>30</v>
       </c>
       <c r="C13" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D13" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E13" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="J13" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="M13" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="T13" t="s">
         <v>36</v>
       </c>
       <c r="U13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="V13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="W13" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="14" spans="1:30" ht="30" x14ac:dyDescent="0.25">
@@ -2594,22 +2570,22 @@
         <v>30</v>
       </c>
       <c r="C14" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D14" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E14" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="J14" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="T14" t="s">
         <v>84</v>
@@ -2632,43 +2608,40 @@
         <v>30</v>
       </c>
       <c r="C15" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D15" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E15" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="J15" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="K15" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="T15" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="U15" t="s">
-        <v>48</v>
+        <v>73</v>
       </c>
       <c r="V15" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="W15" t="s">
-        <v>48</v>
-      </c>
-      <c r="X15" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="AA15" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="AB15" t="s">
         <v>41</v>
@@ -2682,28 +2655,28 @@
         <v>30</v>
       </c>
       <c r="C16" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D16" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E16" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F16" t="s">
         <v>106</v>
       </c>
       <c r="G16" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="J16" t="s">
+        <v>142</v>
+      </c>
+      <c r="K16" t="s">
+        <v>143</v>
+      </c>
+      <c r="R16" t="s">
         <v>141</v>
-      </c>
-      <c r="K16" t="s">
-        <v>142</v>
-      </c>
-      <c r="R16" t="s">
-        <v>140</v>
       </c>
       <c r="T16" t="s">
         <v>36</v>
@@ -2712,13 +2685,13 @@
         <v>37</v>
       </c>
       <c r="V16" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="W16" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="AA16" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="AB16" t="s">
         <v>41</v>
@@ -2732,22 +2705,22 @@
         <v>30</v>
       </c>
       <c r="C17" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D17" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E17" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="J17" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="T17" t="s">
         <v>36</v>
@@ -2759,10 +2732,10 @@
         <v>101</v>
       </c>
       <c r="W17" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="AA17" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="AB17" t="s">
         <v>41</v>
@@ -2776,28 +2749,28 @@
         <v>30</v>
       </c>
       <c r="C18" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D18" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E18" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F18" t="s">
         <v>106</v>
       </c>
       <c r="G18" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="J18" t="s">
+        <v>153</v>
+      </c>
+      <c r="K18" t="s">
+        <v>154</v>
+      </c>
+      <c r="R18" t="s">
         <v>152</v>
-      </c>
-      <c r="K18" t="s">
-        <v>153</v>
-      </c>
-      <c r="R18" t="s">
-        <v>151</v>
       </c>
       <c r="T18" t="s">
         <v>36</v>
@@ -2806,10 +2779,10 @@
         <v>37</v>
       </c>
       <c r="V18" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="W18" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:28" ht="45" x14ac:dyDescent="0.25">
@@ -2820,22 +2793,22 @@
         <v>30</v>
       </c>
       <c r="C19" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D19" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E19" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="F19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="J19" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="T19" t="s">
         <v>36</v>
@@ -2847,10 +2820,10 @@
         <v>101</v>
       </c>
       <c r="W19" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="AA19" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="AB19" t="s">
         <v>41</v>
@@ -2864,28 +2837,28 @@
         <v>30</v>
       </c>
       <c r="C20" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D20" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="E20" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F20" t="s">
         <v>106</v>
       </c>
       <c r="G20" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="J20" t="s">
+        <v>161</v>
+      </c>
+      <c r="K20" t="s">
+        <v>162</v>
+      </c>
+      <c r="R20" t="s">
         <v>160</v>
-      </c>
-      <c r="K20" t="s">
-        <v>161</v>
-      </c>
-      <c r="R20" t="s">
-        <v>159</v>
       </c>
       <c r="T20" t="s">
         <v>36</v>
@@ -2894,10 +2867,10 @@
         <v>37</v>
       </c>
       <c r="V20" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="W20" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:28" x14ac:dyDescent="0.25">
@@ -2908,28 +2881,28 @@
         <v>30</v>
       </c>
       <c r="C21" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D21" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E21" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="F21" t="s">
         <v>106</v>
       </c>
       <c r="G21" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="J21" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="K21" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="R21" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="T21" t="s">
         <v>36</v>
@@ -2938,13 +2911,13 @@
         <v>37</v>
       </c>
       <c r="V21" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="W21" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="AA21" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="AB21" t="s">
         <v>41</v>
@@ -2958,22 +2931,22 @@
         <v>30</v>
       </c>
       <c r="C22" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D22" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E22" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="J22" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="T22" t="s">
         <v>36</v>
@@ -2985,7 +2958,7 @@
         <v>101</v>
       </c>
       <c r="W22" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="23" spans="1:28" x14ac:dyDescent="0.25">
@@ -2996,28 +2969,28 @@
         <v>30</v>
       </c>
       <c r="C23" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D23" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E23" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="F23" t="s">
         <v>106</v>
       </c>
       <c r="G23" t="s">
+        <v>173</v>
+      </c>
+      <c r="J23" t="s">
+        <v>174</v>
+      </c>
+      <c r="K23" t="s">
         <v>172</v>
       </c>
-      <c r="J23" t="s">
+      <c r="R23" t="s">
         <v>173</v>
-      </c>
-      <c r="K23" t="s">
-        <v>171</v>
-      </c>
-      <c r="R23" t="s">
-        <v>172</v>
       </c>
       <c r="T23" t="s">
         <v>36</v>
@@ -3026,10 +2999,10 @@
         <v>37</v>
       </c>
       <c r="V23" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="W23" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:28" ht="60" x14ac:dyDescent="0.25">
@@ -3040,19 +3013,19 @@
         <v>30</v>
       </c>
       <c r="C24" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D24" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E24" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="F24" t="s">
         <v>34</v>
       </c>
       <c r="J24" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="T24" t="s">
         <v>36</v>
@@ -3064,7 +3037,7 @@
         <v>101</v>
       </c>
       <c r="W24" s="1" t="s">
-        <v>419</v>
+        <v>177</v>
       </c>
     </row>
     <row r="25" spans="1:28" x14ac:dyDescent="0.25">
@@ -3075,28 +3048,28 @@
         <v>30</v>
       </c>
       <c r="C25" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="D25" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="E25" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="F25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G25" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="J25" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="K25" t="s">
+        <v>183</v>
+      </c>
+      <c r="R25" t="s">
         <v>181</v>
-      </c>
-      <c r="R25" t="s">
-        <v>179</v>
       </c>
       <c r="T25" t="s">
         <v>36</v>
@@ -3105,10 +3078,10 @@
         <v>37</v>
       </c>
       <c r="V25" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="W25" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:28" x14ac:dyDescent="0.25">
@@ -3119,28 +3092,28 @@
         <v>30</v>
       </c>
       <c r="C26" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="D26" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="E26" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="F26" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G26" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="J26" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="K26" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="R26" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="T26" t="s">
         <v>36</v>
@@ -3149,13 +3122,13 @@
         <v>37</v>
       </c>
       <c r="V26" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="W26" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="27" spans="1:28" ht="90" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="1:28" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3163,40 +3136,40 @@
         <v>30</v>
       </c>
       <c r="C27" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="D27" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="E27" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="F27" t="s">
         <v>106</v>
       </c>
       <c r="G27" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="R27" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="T27" t="s">
         <v>36</v>
       </c>
       <c r="U27" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="V27" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="W27" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
     </row>
     <row r="28" spans="1:28" x14ac:dyDescent="0.25">
@@ -3207,25 +3180,25 @@
         <v>30</v>
       </c>
       <c r="C28" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="D28" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="E28" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="F28" t="s">
         <v>106</v>
       </c>
       <c r="G28" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="J28" t="s">
-        <v>411</v>
+        <v>200</v>
       </c>
       <c r="S28" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="T28" t="s">
         <v>36</v>
@@ -3234,13 +3207,13 @@
         <v>37</v>
       </c>
       <c r="V28" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="W28" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="X28" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
     </row>
     <row r="29" spans="1:28" ht="45" x14ac:dyDescent="0.25">
@@ -3251,34 +3224,34 @@
         <v>30</v>
       </c>
       <c r="C29" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="D29" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="E29" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="F29" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="J29" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="T29" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="U29" t="s">
-        <v>48</v>
+        <v>207</v>
       </c>
       <c r="V29" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="W29" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
     </row>
     <row r="30" spans="1:28" x14ac:dyDescent="0.25">
@@ -3289,28 +3262,28 @@
         <v>30</v>
       </c>
       <c r="C30" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="D30" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="E30" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="F30" t="s">
         <v>106</v>
       </c>
       <c r="G30" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="J30" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="K30" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="R30" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="T30" t="s">
         <v>36</v>
@@ -3319,10 +3292,10 @@
         <v>37</v>
       </c>
       <c r="V30" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="W30" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
     </row>
     <row r="31" spans="1:28" x14ac:dyDescent="0.25">
@@ -3333,22 +3306,22 @@
         <v>30</v>
       </c>
       <c r="C31" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="D31" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="E31" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="F31" t="s">
         <v>106</v>
       </c>
       <c r="G31" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="J31" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="T31" t="s">
         <v>84</v>
@@ -3371,22 +3344,22 @@
         <v>30</v>
       </c>
       <c r="C32" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="D32" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="E32" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="F32" t="s">
         <v>106</v>
       </c>
       <c r="G32" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="J32" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="T32" t="s">
         <v>84</v>
@@ -3409,22 +3382,22 @@
         <v>30</v>
       </c>
       <c r="C33" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="D33" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="E33" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="F33" t="s">
         <v>106</v>
       </c>
       <c r="G33" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="J33" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="T33" t="s">
         <v>84</v>
@@ -3447,22 +3420,22 @@
         <v>30</v>
       </c>
       <c r="C34" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="D34" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="E34" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="F34" t="s">
         <v>106</v>
       </c>
       <c r="G34" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="J34" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="T34" t="s">
         <v>84</v>
@@ -3485,22 +3458,22 @@
         <v>30</v>
       </c>
       <c r="C35" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="D35" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="E35" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="F35" t="s">
         <v>106</v>
       </c>
       <c r="G35" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="J35" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="T35" t="s">
         <v>84</v>
@@ -3523,22 +3496,22 @@
         <v>30</v>
       </c>
       <c r="C36" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="D36" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="E36" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="F36" t="s">
         <v>106</v>
       </c>
       <c r="G36" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="J36" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="T36" t="s">
         <v>84</v>
@@ -3561,22 +3534,22 @@
         <v>30</v>
       </c>
       <c r="C37" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="D37" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="E37" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="F37" t="s">
         <v>106</v>
       </c>
       <c r="G37" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="J37" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="T37" t="s">
         <v>84</v>
@@ -3599,22 +3572,22 @@
         <v>30</v>
       </c>
       <c r="C38" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="D38" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="E38" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="F38" t="s">
         <v>106</v>
       </c>
       <c r="G38" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="J38" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="T38" t="s">
         <v>84</v>
@@ -3637,22 +3610,22 @@
         <v>30</v>
       </c>
       <c r="C39" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="D39" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="E39" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="F39" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="J39" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="T39" t="s">
         <v>84</v>
@@ -3675,22 +3648,22 @@
         <v>30</v>
       </c>
       <c r="C40" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="D40" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="E40" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="F40" t="s">
         <v>106</v>
       </c>
       <c r="G40" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="J40" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="T40" t="s">
         <v>84</v>
@@ -3713,22 +3686,22 @@
         <v>30</v>
       </c>
       <c r="C41" t="s">
+        <v>241</v>
+      </c>
+      <c r="D41" t="s">
+        <v>242</v>
+      </c>
+      <c r="E41" t="s">
+        <v>243</v>
+      </c>
+      <c r="F41" t="s">
+        <v>55</v>
+      </c>
+      <c r="I41" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="D41" t="s">
-        <v>238</v>
-      </c>
-      <c r="E41" t="s">
-        <v>239</v>
-      </c>
-      <c r="F41" t="s">
-        <v>56</v>
-      </c>
-      <c r="I41" s="1" t="s">
-        <v>233</v>
-      </c>
       <c r="J41" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="T41" t="s">
         <v>84</v>
@@ -3751,22 +3724,22 @@
         <v>30</v>
       </c>
       <c r="C42" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="D42" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="E42" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="F42" t="s">
         <v>106</v>
       </c>
       <c r="G42" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="J42" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="T42" t="s">
         <v>84</v>
@@ -3781,7 +3754,7 @@
         <v>84</v>
       </c>
       <c r="AA42" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="AB42" t="s">
         <v>41</v>
@@ -3795,46 +3768,46 @@
         <v>30</v>
       </c>
       <c r="C43" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="D43" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="E43" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="F43" t="s">
         <v>106</v>
       </c>
       <c r="G43" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="J43" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="K43" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="Q43" s="1" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="S43" s="1" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="T43" t="s">
         <v>36</v>
       </c>
       <c r="U43" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="V43" t="s">
         <v>101</v>
       </c>
       <c r="W43" s="1" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="AA43" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="AB43" t="s">
         <v>41</v>
@@ -3848,40 +3821,40 @@
         <v>30</v>
       </c>
       <c r="C44" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="D44" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="E44" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="F44" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="J44" s="1" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="Q44" s="1" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="T44" t="s">
         <v>36</v>
       </c>
       <c r="U44" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="V44" t="s">
         <v>101</v>
       </c>
       <c r="W44" s="1" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="45" spans="1:28" ht="120" x14ac:dyDescent="0.25">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="45" spans="1:28" ht="45" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -3889,46 +3862,37 @@
         <v>30</v>
       </c>
       <c r="C45" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="D45" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="E45" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="F45" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="J45" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="K45" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="Q45" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
+      </c>
+      <c r="J45" t="s">
+        <v>83</v>
       </c>
       <c r="T45" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="U45" t="s">
-        <v>48</v>
+        <v>85</v>
       </c>
       <c r="V45" t="s">
-        <v>48</v>
-      </c>
-      <c r="W45" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="X45" s="1" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="46" spans="1:28" ht="150" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+      <c r="W45" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="46" spans="1:28" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -3945,7 +3909,7 @@
         <v>269</v>
       </c>
       <c r="F46" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I46" s="1" t="s">
         <v>270</v>
@@ -3963,10 +3927,10 @@
         <v>36</v>
       </c>
       <c r="U46" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="V46" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="W46" t="s">
         <v>274</v>
@@ -3992,7 +3956,7 @@
         <v>277</v>
       </c>
       <c r="F47" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G47" t="s">
         <v>278</v>
@@ -4007,7 +3971,7 @@
         <v>36</v>
       </c>
       <c r="U47" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="V47" t="s">
         <v>101</v>
@@ -4033,7 +3997,7 @@
         <v>283</v>
       </c>
       <c r="F48" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I48" s="1" t="s">
         <v>284</v>
@@ -4051,10 +4015,10 @@
         <v>36</v>
       </c>
       <c r="U48" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="V48" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="W48" t="s">
         <v>288</v>
@@ -4077,13 +4041,13 @@
         <v>291</v>
       </c>
       <c r="F49" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I49" s="1" t="s">
         <v>292</v>
       </c>
       <c r="J49" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="T49" t="s">
         <v>84</v>
@@ -4115,13 +4079,13 @@
         <v>295</v>
       </c>
       <c r="F50" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I50" s="1" t="s">
         <v>292</v>
       </c>
       <c r="J50" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="T50" t="s">
         <v>84</v>
@@ -4153,13 +4117,13 @@
         <v>297</v>
       </c>
       <c r="F51" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I51" s="1" t="s">
         <v>292</v>
       </c>
       <c r="J51" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="T51" t="s">
         <v>84</v>
@@ -4191,13 +4155,13 @@
         <v>299</v>
       </c>
       <c r="F52" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I52" s="1" t="s">
         <v>300</v>
       </c>
       <c r="J52" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="T52" t="s">
         <v>84</v>
@@ -4229,13 +4193,13 @@
         <v>302</v>
       </c>
       <c r="F53" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I53" s="1" t="s">
         <v>292</v>
       </c>
       <c r="J53" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="T53" t="s">
         <v>84</v>
@@ -4267,13 +4231,13 @@
         <v>304</v>
       </c>
       <c r="F54" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I54" s="1" t="s">
         <v>292</v>
       </c>
       <c r="J54" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="T54" t="s">
         <v>84</v>
@@ -4305,13 +4269,13 @@
         <v>306</v>
       </c>
       <c r="F55" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I55" s="1" t="s">
         <v>292</v>
       </c>
       <c r="J55" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="T55" t="s">
         <v>84</v>
@@ -4343,13 +4307,13 @@
         <v>308</v>
       </c>
       <c r="F56" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I56" s="1" t="s">
         <v>292</v>
       </c>
       <c r="J56" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="T56" t="s">
         <v>84</v>
@@ -4387,13 +4351,13 @@
         <v>311</v>
       </c>
       <c r="F57" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I57" s="1" t="s">
         <v>292</v>
       </c>
       <c r="J57" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="T57" t="s">
         <v>84</v>
@@ -4425,13 +4389,13 @@
         <v>314</v>
       </c>
       <c r="F58" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I58" s="1" t="s">
         <v>292</v>
       </c>
       <c r="J58" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="T58" t="s">
         <v>84</v>
@@ -4463,10 +4427,10 @@
         <v>316</v>
       </c>
       <c r="F59" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J59" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="T59" t="s">
         <v>84</v>
@@ -4498,10 +4462,10 @@
         <v>318</v>
       </c>
       <c r="F60" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J60" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="T60" t="s">
         <v>84</v>
@@ -4533,10 +4497,10 @@
         <v>320</v>
       </c>
       <c r="F61" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J61" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="T61" t="s">
         <v>84</v>
@@ -4568,10 +4532,10 @@
         <v>322</v>
       </c>
       <c r="F62" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J62" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="T62" t="s">
         <v>84</v>
@@ -4603,10 +4567,10 @@
         <v>324</v>
       </c>
       <c r="F63" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J63" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="T63" t="s">
         <v>84</v>
@@ -4638,10 +4602,10 @@
         <v>326</v>
       </c>
       <c r="F64" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J64" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="T64" t="s">
         <v>84</v>
@@ -4673,10 +4637,10 @@
         <v>328</v>
       </c>
       <c r="F65" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J65" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="T65" t="s">
         <v>84</v>
@@ -4691,7 +4655,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="66" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
@@ -4708,13 +4672,13 @@
         <v>330</v>
       </c>
       <c r="F66" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I66" s="1" t="s">
         <v>331</v>
       </c>
       <c r="J66" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="T66" t="s">
         <v>84</v>
@@ -4752,7 +4716,7 @@
         <v>334</v>
       </c>
       <c r="J67" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="T67" t="s">
         <v>84</v>
@@ -4784,13 +4748,13 @@
         <v>336</v>
       </c>
       <c r="F68" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I68" s="1" t="s">
         <v>337</v>
       </c>
       <c r="J68" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="T68" t="s">
         <v>84</v>
@@ -4822,7 +4786,7 @@
         <v>339</v>
       </c>
       <c r="F69" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I69" s="1" t="s">
         <v>340</v>
@@ -4837,16 +4801,16 @@
         <v>37</v>
       </c>
       <c r="V69" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="W69" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="X69" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="70" spans="1:24" ht="150" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:24" ht="180" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
@@ -4863,7 +4827,7 @@
         <v>344</v>
       </c>
       <c r="F70" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I70" s="1" t="s">
         <v>345</v>
@@ -4881,13 +4845,13 @@
         <v>36</v>
       </c>
       <c r="U70" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="V70" t="s">
         <v>101</v>
       </c>
       <c r="W70" s="1" t="s">
-        <v>412</v>
+        <v>349</v>
       </c>
     </row>
     <row r="71" spans="1:24" ht="90" x14ac:dyDescent="0.25">
@@ -4898,40 +4862,40 @@
         <v>30</v>
       </c>
       <c r="C71" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="D71" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="E71" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="F71" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I71" s="1" t="s">
         <v>345</v>
       </c>
       <c r="J71" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="K71" t="s">
         <v>347</v>
       </c>
       <c r="M71" s="1" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="T71" t="s">
         <v>36</v>
       </c>
       <c r="U71" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="V71" t="s">
         <v>101</v>
       </c>
       <c r="W71" s="1" t="s">
-        <v>413</v>
+        <v>354</v>
       </c>
     </row>
     <row r="72" spans="1:24" ht="90" x14ac:dyDescent="0.25">
@@ -4942,40 +4906,40 @@
         <v>30</v>
       </c>
       <c r="C72" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="D72" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="E72" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="F72" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I72" s="1" t="s">
         <v>345</v>
       </c>
       <c r="J72" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="K72" t="s">
         <v>347</v>
       </c>
       <c r="M72" s="1" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="T72" t="s">
         <v>36</v>
       </c>
       <c r="U72" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="V72" t="s">
         <v>101</v>
       </c>
       <c r="W72" s="1" t="s">
-        <v>414</v>
+        <v>359</v>
       </c>
     </row>
     <row r="73" spans="1:24" ht="165" x14ac:dyDescent="0.25">
@@ -4986,28 +4950,28 @@
         <v>30</v>
       </c>
       <c r="C73" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="D73" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
       <c r="E73" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="F73" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
       <c r="J73" s="1" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="T73" t="s">
         <v>84</v>
       </c>
       <c r="U73" t="s">
-        <v>362</v>
+        <v>207</v>
       </c>
       <c r="V73" t="s">
         <v>84</v>
@@ -5016,10 +4980,10 @@
         <v>84</v>
       </c>
       <c r="X73" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="74" spans="1:24" ht="195" x14ac:dyDescent="0.25">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="74" spans="1:24" ht="210" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
@@ -5027,25 +4991,25 @@
         <v>30</v>
       </c>
       <c r="C74" t="s">
+        <v>366</v>
+      </c>
+      <c r="D74" t="s">
+        <v>367</v>
+      </c>
+      <c r="E74" t="s">
+        <v>368</v>
+      </c>
+      <c r="F74" t="s">
+        <v>55</v>
+      </c>
+      <c r="I74" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="J74" s="1" t="s">
         <v>364</v>
       </c>
-      <c r="D74" t="s">
-        <v>365</v>
-      </c>
-      <c r="E74" t="s">
-        <v>366</v>
-      </c>
-      <c r="F74" t="s">
-        <v>56</v>
-      </c>
-      <c r="I74" s="1" t="s">
-        <v>367</v>
-      </c>
-      <c r="J74" s="1" t="s">
-        <v>361</v>
-      </c>
       <c r="K74" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="M74" s="1" t="s">
         <v>348</v>
@@ -5054,16 +5018,16 @@
         <v>36</v>
       </c>
       <c r="U74" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="V74" t="s">
         <v>101</v>
       </c>
       <c r="W74" s="1" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="75" spans="1:24" ht="150" x14ac:dyDescent="0.25">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="75" spans="1:24" ht="195" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
@@ -5071,25 +5035,25 @@
         <v>30</v>
       </c>
       <c r="C75" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
       <c r="D75" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="E75" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="F75" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I75" s="1" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="J75" s="1" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
       <c r="K75" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="M75" s="1" t="s">
         <v>348</v>
@@ -5098,16 +5062,16 @@
         <v>36</v>
       </c>
       <c r="U75" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="V75" t="s">
         <v>101</v>
       </c>
       <c r="W75" s="1" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="76" spans="1:24" ht="135" x14ac:dyDescent="0.25">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="76" spans="1:24" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
@@ -5115,46 +5079,46 @@
         <v>30</v>
       </c>
       <c r="C76" t="s">
-        <v>375</v>
+        <v>379</v>
       </c>
       <c r="D76" t="s">
-        <v>376</v>
+        <v>380</v>
       </c>
       <c r="E76" t="s">
-        <v>377</v>
+        <v>381</v>
       </c>
       <c r="F76" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G76" t="s">
         <v>334</v>
       </c>
       <c r="J76" t="s">
-        <v>378</v>
+        <v>382</v>
       </c>
       <c r="K76" s="1" t="s">
-        <v>379</v>
+        <v>383</v>
       </c>
       <c r="Q76" t="s">
-        <v>380</v>
+        <v>384</v>
       </c>
       <c r="T76" t="s">
         <v>36</v>
       </c>
       <c r="U76" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="V76" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="W76" t="s">
-        <v>418</v>
+        <v>385</v>
       </c>
       <c r="X76" s="1" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="77" spans="1:24" ht="165" x14ac:dyDescent="0.25">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="77" spans="1:24" ht="195" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
@@ -5162,40 +5126,40 @@
         <v>30</v>
       </c>
       <c r="C77" t="s">
+        <v>387</v>
+      </c>
+      <c r="D77" t="s">
+        <v>388</v>
+      </c>
+      <c r="E77" t="s">
+        <v>389</v>
+      </c>
+      <c r="F77" t="s">
+        <v>55</v>
+      </c>
+      <c r="I77" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="J77" t="s">
         <v>382</v>
       </c>
-      <c r="D77" t="s">
-        <v>383</v>
-      </c>
-      <c r="E77" t="s">
+      <c r="K77" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="Q77" t="s">
         <v>384</v>
-      </c>
-      <c r="F77" t="s">
-        <v>56</v>
-      </c>
-      <c r="I77" s="1" t="s">
-        <v>385</v>
-      </c>
-      <c r="J77" t="s">
-        <v>378</v>
-      </c>
-      <c r="K77" s="1" t="s">
-        <v>386</v>
-      </c>
-      <c r="Q77" t="s">
-        <v>380</v>
       </c>
       <c r="T77" t="s">
         <v>36</v>
       </c>
       <c r="U77" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="V77" t="s">
         <v>101</v>
       </c>
       <c r="W77" s="1" t="s">
-        <v>417</v>
+        <v>392</v>
       </c>
     </row>
     <row r="78" spans="1:24" ht="45" x14ac:dyDescent="0.25">
@@ -5206,22 +5170,22 @@
         <v>30</v>
       </c>
       <c r="C78" t="s">
-        <v>387</v>
+        <v>393</v>
       </c>
       <c r="D78" t="s">
-        <v>388</v>
+        <v>394</v>
       </c>
       <c r="E78" t="s">
-        <v>389</v>
+        <v>395</v>
       </c>
       <c r="F78" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I78" s="1" t="s">
-        <v>390</v>
+        <v>396</v>
       </c>
       <c r="J78" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="T78" t="s">
         <v>84</v>
@@ -5236,7 +5200,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="79" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
@@ -5244,22 +5208,22 @@
         <v>30</v>
       </c>
       <c r="C79" t="s">
-        <v>391</v>
+        <v>397</v>
       </c>
       <c r="D79" t="s">
-        <v>392</v>
+        <v>398</v>
       </c>
       <c r="E79" t="s">
-        <v>392</v>
+        <v>398</v>
       </c>
       <c r="F79" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I79" s="1" t="s">
-        <v>393</v>
+        <v>399</v>
       </c>
       <c r="J79" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="T79" t="s">
         <v>84</v>
@@ -5282,22 +5246,22 @@
         <v>30</v>
       </c>
       <c r="C80" t="s">
-        <v>394</v>
+        <v>400</v>
       </c>
       <c r="D80" t="s">
-        <v>395</v>
+        <v>401</v>
       </c>
       <c r="E80" t="s">
-        <v>396</v>
+        <v>402</v>
       </c>
       <c r="F80" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I80" s="1" t="s">
         <v>292</v>
       </c>
       <c r="J80" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="T80" t="s">
         <v>84</v>
@@ -5320,22 +5284,22 @@
         <v>30</v>
       </c>
       <c r="C81" t="s">
-        <v>397</v>
+        <v>403</v>
       </c>
       <c r="D81" t="s">
-        <v>398</v>
+        <v>404</v>
       </c>
       <c r="E81" t="s">
-        <v>399</v>
+        <v>405</v>
       </c>
       <c r="F81" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I81" s="1" t="s">
         <v>292</v>
       </c>
       <c r="J81" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="T81" t="s">
         <v>84</v>
@@ -5358,22 +5322,22 @@
         <v>30</v>
       </c>
       <c r="C82" t="s">
-        <v>400</v>
+        <v>406</v>
       </c>
       <c r="D82" t="s">
-        <v>401</v>
+        <v>407</v>
       </c>
       <c r="E82" t="s">
-        <v>402</v>
+        <v>408</v>
       </c>
       <c r="F82" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I82" s="1" t="s">
         <v>292</v>
       </c>
       <c r="J82" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="T82" t="s">
         <v>84</v>
@@ -5396,19 +5360,19 @@
         <v>30</v>
       </c>
       <c r="C83" t="s">
-        <v>403</v>
+        <v>409</v>
       </c>
       <c r="D83" t="s">
-        <v>404</v>
+        <v>410</v>
       </c>
       <c r="E83" t="s">
-        <v>405</v>
+        <v>411</v>
       </c>
       <c r="F83" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J83" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="T83" t="s">
         <v>84</v>
@@ -5431,22 +5395,22 @@
         <v>30</v>
       </c>
       <c r="C84" t="s">
-        <v>406</v>
+        <v>412</v>
       </c>
       <c r="D84" t="s">
-        <v>407</v>
+        <v>413</v>
       </c>
       <c r="E84" t="s">
-        <v>408</v>
+        <v>414</v>
       </c>
       <c r="F84" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G84" t="s">
-        <v>409</v>
+        <v>415</v>
       </c>
       <c r="J84" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="T84" t="s">
         <v>84</v>
@@ -5463,6 +5427,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
correct typo sdc_location variable harmo rule
</commit_message>
<xml_diff>
--- a/data_processing_elements-HBS.xlsx
+++ b/data_processing_elements-HBS.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/849507f40a0f895e/Documents/ProPASS/Studies/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbtiali\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{09B0DEE3-935C-46B5-B8C0-152FC6679B3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{500F5325-7AB5-4997-8FD4-C7140FEB5B95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{AA860D54-F729-477E-8EFC-6CB92CB671B4}"/>
   </bookViews>
@@ -545,9 +545,6 @@
     <t>You live in</t>
   </si>
   <si>
-    <t>recode(1=2; 2=1; ELSE=NA_integer)</t>
-  </si>
-  <si>
     <t>All participants reside in Soweto, an urban area</t>
   </si>
   <si>
@@ -1530,6 +1527,9 @@
   </si>
   <si>
     <t>items</t>
+  </si>
+  <si>
+    <t>recode(1=2; 2=1; ELSE=NA_integer_)</t>
   </si>
 </sst>
 </file>
@@ -1915,8 +1915,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5FD0B37-B6E8-454F-93F7-57FF9B64A4BB}">
   <dimension ref="A1:AD84"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView tabSelected="1" topLeftCell="M12" workbookViewId="0">
+      <selection activeCell="W16" sqref="W16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2638,10 +2638,10 @@
         <v>59</v>
       </c>
       <c r="W15" t="s">
+        <v>415</v>
+      </c>
+      <c r="AA15" t="s">
         <v>137</v>
-      </c>
-      <c r="AA15" t="s">
-        <v>138</v>
       </c>
       <c r="AB15" t="s">
         <v>41</v>
@@ -2655,28 +2655,28 @@
         <v>30</v>
       </c>
       <c r="C16" t="s">
+        <v>138</v>
+      </c>
+      <c r="D16" t="s">
         <v>139</v>
       </c>
-      <c r="D16" t="s">
-        <v>140</v>
-      </c>
       <c r="E16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F16" t="s">
         <v>106</v>
       </c>
       <c r="G16" t="s">
+        <v>140</v>
+      </c>
+      <c r="J16" t="s">
         <v>141</v>
       </c>
-      <c r="J16" t="s">
+      <c r="K16" t="s">
         <v>142</v>
       </c>
-      <c r="K16" t="s">
-        <v>143</v>
-      </c>
       <c r="R16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="T16" t="s">
         <v>36</v>
@@ -2691,7 +2691,7 @@
         <v>47</v>
       </c>
       <c r="AA16" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="AB16" t="s">
         <v>41</v>
@@ -2705,22 +2705,22 @@
         <v>30</v>
       </c>
       <c r="C17" t="s">
+        <v>144</v>
+      </c>
+      <c r="D17" t="s">
         <v>145</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
+        <v>145</v>
+      </c>
+      <c r="F17" t="s">
+        <v>55</v>
+      </c>
+      <c r="I17" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="E17" t="s">
-        <v>146</v>
-      </c>
-      <c r="F17" t="s">
-        <v>55</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>147</v>
-      </c>
       <c r="J17" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="T17" t="s">
         <v>36</v>
@@ -2732,10 +2732,10 @@
         <v>101</v>
       </c>
       <c r="W17" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="AA17" t="s">
         <v>148</v>
-      </c>
-      <c r="AA17" t="s">
-        <v>149</v>
       </c>
       <c r="AB17" t="s">
         <v>41</v>
@@ -2749,28 +2749,28 @@
         <v>30</v>
       </c>
       <c r="C18" t="s">
+        <v>149</v>
+      </c>
+      <c r="D18" t="s">
         <v>150</v>
       </c>
-      <c r="D18" t="s">
-        <v>151</v>
-      </c>
       <c r="E18" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F18" t="s">
         <v>106</v>
       </c>
       <c r="G18" t="s">
+        <v>151</v>
+      </c>
+      <c r="J18" t="s">
         <v>152</v>
       </c>
-      <c r="J18" t="s">
+      <c r="K18" t="s">
         <v>153</v>
       </c>
-      <c r="K18" t="s">
-        <v>154</v>
-      </c>
       <c r="R18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="T18" t="s">
         <v>36</v>
@@ -2793,22 +2793,22 @@
         <v>30</v>
       </c>
       <c r="C19" t="s">
+        <v>154</v>
+      </c>
+      <c r="D19" t="s">
         <v>155</v>
       </c>
-      <c r="D19" t="s">
-        <v>156</v>
-      </c>
       <c r="E19" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F19" t="s">
         <v>55</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J19" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="T19" t="s">
         <v>36</v>
@@ -2820,10 +2820,10 @@
         <v>101</v>
       </c>
       <c r="W19" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AA19" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="AB19" t="s">
         <v>41</v>
@@ -2837,28 +2837,28 @@
         <v>30</v>
       </c>
       <c r="C20" t="s">
+        <v>157</v>
+      </c>
+      <c r="D20" t="s">
         <v>158</v>
       </c>
-      <c r="D20" t="s">
-        <v>159</v>
-      </c>
       <c r="E20" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F20" t="s">
         <v>106</v>
       </c>
       <c r="G20" t="s">
+        <v>159</v>
+      </c>
+      <c r="J20" t="s">
         <v>160</v>
       </c>
-      <c r="J20" t="s">
+      <c r="K20" t="s">
         <v>161</v>
       </c>
-      <c r="K20" t="s">
-        <v>162</v>
-      </c>
       <c r="R20" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="T20" t="s">
         <v>36</v>
@@ -2881,28 +2881,28 @@
         <v>30</v>
       </c>
       <c r="C21" t="s">
+        <v>162</v>
+      </c>
+      <c r="D21" t="s">
         <v>163</v>
       </c>
-      <c r="D21" t="s">
-        <v>164</v>
-      </c>
       <c r="E21" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F21" t="s">
         <v>106</v>
       </c>
       <c r="G21" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J21" t="s">
+        <v>164</v>
+      </c>
+      <c r="K21" t="s">
         <v>165</v>
       </c>
-      <c r="K21" t="s">
-        <v>166</v>
-      </c>
       <c r="R21" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="T21" t="s">
         <v>36</v>
@@ -2917,7 +2917,7 @@
         <v>47</v>
       </c>
       <c r="AA21" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="AB21" t="s">
         <v>41</v>
@@ -2931,22 +2931,22 @@
         <v>30</v>
       </c>
       <c r="C22" t="s">
+        <v>167</v>
+      </c>
+      <c r="D22" t="s">
         <v>168</v>
       </c>
-      <c r="D22" t="s">
-        <v>169</v>
-      </c>
       <c r="E22" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F22" t="s">
         <v>55</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J22" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="T22" t="s">
         <v>36</v>
@@ -2958,7 +2958,7 @@
         <v>101</v>
       </c>
       <c r="W22" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="23" spans="1:28" x14ac:dyDescent="0.25">
@@ -2969,28 +2969,28 @@
         <v>30</v>
       </c>
       <c r="C23" t="s">
+        <v>170</v>
+      </c>
+      <c r="D23" t="s">
         <v>171</v>
       </c>
-      <c r="D23" t="s">
-        <v>172</v>
-      </c>
       <c r="E23" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F23" t="s">
         <v>106</v>
       </c>
       <c r="G23" t="s">
+        <v>172</v>
+      </c>
+      <c r="J23" t="s">
         <v>173</v>
       </c>
-      <c r="J23" t="s">
-        <v>174</v>
-      </c>
       <c r="K23" t="s">
+        <v>171</v>
+      </c>
+      <c r="R23" t="s">
         <v>172</v>
-      </c>
-      <c r="R23" t="s">
-        <v>173</v>
       </c>
       <c r="T23" t="s">
         <v>36</v>
@@ -3013,19 +3013,19 @@
         <v>30</v>
       </c>
       <c r="C24" t="s">
+        <v>174</v>
+      </c>
+      <c r="D24" t="s">
         <v>175</v>
       </c>
-      <c r="D24" t="s">
-        <v>176</v>
-      </c>
       <c r="E24" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F24" t="s">
         <v>34</v>
       </c>
       <c r="J24" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="T24" t="s">
         <v>36</v>
@@ -3037,7 +3037,7 @@
         <v>101</v>
       </c>
       <c r="W24" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="25" spans="1:28" x14ac:dyDescent="0.25">
@@ -3048,28 +3048,28 @@
         <v>30</v>
       </c>
       <c r="C25" t="s">
+        <v>177</v>
+      </c>
+      <c r="D25" t="s">
         <v>178</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>179</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
+        <v>55</v>
+      </c>
+      <c r="G25" t="s">
         <v>180</v>
       </c>
-      <c r="F25" t="s">
-        <v>55</v>
-      </c>
-      <c r="G25" t="s">
+      <c r="J25" t="s">
         <v>181</v>
       </c>
-      <c r="J25" t="s">
+      <c r="K25" t="s">
         <v>182</v>
       </c>
-      <c r="K25" t="s">
-        <v>183</v>
-      </c>
       <c r="R25" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="T25" t="s">
         <v>36</v>
@@ -3092,28 +3092,28 @@
         <v>30</v>
       </c>
       <c r="C26" t="s">
+        <v>183</v>
+      </c>
+      <c r="D26" t="s">
         <v>184</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>185</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
+        <v>55</v>
+      </c>
+      <c r="G26" t="s">
+        <v>180</v>
+      </c>
+      <c r="J26" t="s">
         <v>186</v>
       </c>
-      <c r="F26" t="s">
-        <v>55</v>
-      </c>
-      <c r="G26" t="s">
-        <v>181</v>
-      </c>
-      <c r="J26" t="s">
+      <c r="K26" t="s">
         <v>187</v>
       </c>
-      <c r="K26" t="s">
-        <v>188</v>
-      </c>
       <c r="R26" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="T26" t="s">
         <v>36</v>
@@ -3136,28 +3136,28 @@
         <v>30</v>
       </c>
       <c r="C27" t="s">
+        <v>188</v>
+      </c>
+      <c r="D27" t="s">
         <v>189</v>
       </c>
-      <c r="D27" t="s">
-        <v>190</v>
-      </c>
       <c r="E27" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F27" t="s">
         <v>106</v>
       </c>
       <c r="G27" t="s">
+        <v>190</v>
+      </c>
+      <c r="J27" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="J27" s="1" t="s">
+      <c r="K27" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="K27" s="1" t="s">
+      <c r="R27" t="s">
         <v>193</v>
-      </c>
-      <c r="R27" t="s">
-        <v>194</v>
       </c>
       <c r="T27" t="s">
         <v>36</v>
@@ -3166,10 +3166,10 @@
         <v>73</v>
       </c>
       <c r="V27" t="s">
+        <v>194</v>
+      </c>
+      <c r="W27" t="s">
         <v>195</v>
-      </c>
-      <c r="W27" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="28" spans="1:28" x14ac:dyDescent="0.25">
@@ -3180,25 +3180,25 @@
         <v>30</v>
       </c>
       <c r="C28" t="s">
+        <v>196</v>
+      </c>
+      <c r="D28" t="s">
         <v>197</v>
       </c>
-      <c r="D28" t="s">
-        <v>198</v>
-      </c>
       <c r="E28" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F28" t="s">
         <v>106</v>
       </c>
       <c r="G28" t="s">
+        <v>198</v>
+      </c>
+      <c r="J28" t="s">
         <v>199</v>
       </c>
-      <c r="J28" t="s">
+      <c r="S28" t="s">
         <v>200</v>
-      </c>
-      <c r="S28" t="s">
-        <v>201</v>
       </c>
       <c r="T28" t="s">
         <v>36</v>
@@ -3213,7 +3213,7 @@
         <v>47</v>
       </c>
       <c r="X28" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="29" spans="1:28" ht="45" x14ac:dyDescent="0.25">
@@ -3224,28 +3224,28 @@
         <v>30</v>
       </c>
       <c r="C29" t="s">
+        <v>202</v>
+      </c>
+      <c r="D29" t="s">
         <v>203</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
+        <v>203</v>
+      </c>
+      <c r="F29" t="s">
+        <v>55</v>
+      </c>
+      <c r="I29" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="E29" t="s">
-        <v>204</v>
-      </c>
-      <c r="F29" t="s">
-        <v>55</v>
-      </c>
-      <c r="I29" s="1" t="s">
+      <c r="J29" t="s">
         <v>205</v>
       </c>
-      <c r="J29" t="s">
+      <c r="T29" t="s">
+        <v>84</v>
+      </c>
+      <c r="U29" t="s">
         <v>206</v>
-      </c>
-      <c r="T29" t="s">
-        <v>84</v>
-      </c>
-      <c r="U29" t="s">
-        <v>207</v>
       </c>
       <c r="V29" t="s">
         <v>84</v>
@@ -3262,28 +3262,28 @@
         <v>30</v>
       </c>
       <c r="C30" t="s">
+        <v>207</v>
+      </c>
+      <c r="D30" t="s">
         <v>208</v>
       </c>
-      <c r="D30" t="s">
-        <v>209</v>
-      </c>
       <c r="E30" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F30" t="s">
         <v>106</v>
       </c>
       <c r="G30" t="s">
+        <v>209</v>
+      </c>
+      <c r="J30" t="s">
         <v>210</v>
       </c>
-      <c r="J30" t="s">
+      <c r="K30" t="s">
         <v>211</v>
       </c>
-      <c r="K30" t="s">
-        <v>212</v>
-      </c>
       <c r="R30" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="T30" t="s">
         <v>36</v>
@@ -3306,19 +3306,19 @@
         <v>30</v>
       </c>
       <c r="C31" t="s">
+        <v>212</v>
+      </c>
+      <c r="D31" t="s">
         <v>213</v>
       </c>
-      <c r="D31" t="s">
-        <v>214</v>
-      </c>
       <c r="E31" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F31" t="s">
         <v>106</v>
       </c>
       <c r="G31" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="J31" t="s">
         <v>83</v>
@@ -3344,19 +3344,19 @@
         <v>30</v>
       </c>
       <c r="C32" t="s">
+        <v>215</v>
+      </c>
+      <c r="D32" t="s">
         <v>216</v>
       </c>
-      <c r="D32" t="s">
-        <v>217</v>
-      </c>
       <c r="E32" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F32" t="s">
         <v>106</v>
       </c>
       <c r="G32" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J32" t="s">
         <v>83</v>
@@ -3382,19 +3382,19 @@
         <v>30</v>
       </c>
       <c r="C33" t="s">
+        <v>218</v>
+      </c>
+      <c r="D33" t="s">
         <v>219</v>
       </c>
-      <c r="D33" t="s">
-        <v>220</v>
-      </c>
       <c r="E33" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F33" t="s">
         <v>106</v>
       </c>
       <c r="G33" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J33" t="s">
         <v>83</v>
@@ -3420,19 +3420,19 @@
         <v>30</v>
       </c>
       <c r="C34" t="s">
+        <v>220</v>
+      </c>
+      <c r="D34" t="s">
         <v>221</v>
       </c>
-      <c r="D34" t="s">
-        <v>222</v>
-      </c>
       <c r="E34" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F34" t="s">
         <v>106</v>
       </c>
       <c r="G34" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J34" t="s">
         <v>83</v>
@@ -3458,19 +3458,19 @@
         <v>30</v>
       </c>
       <c r="C35" t="s">
+        <v>222</v>
+      </c>
+      <c r="D35" t="s">
         <v>223</v>
       </c>
-      <c r="D35" t="s">
-        <v>224</v>
-      </c>
       <c r="E35" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F35" t="s">
         <v>106</v>
       </c>
       <c r="G35" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J35" t="s">
         <v>83</v>
@@ -3496,19 +3496,19 @@
         <v>30</v>
       </c>
       <c r="C36" t="s">
+        <v>224</v>
+      </c>
+      <c r="D36" t="s">
         <v>225</v>
       </c>
-      <c r="D36" t="s">
-        <v>226</v>
-      </c>
       <c r="E36" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F36" t="s">
         <v>106</v>
       </c>
       <c r="G36" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J36" t="s">
         <v>83</v>
@@ -3534,19 +3534,19 @@
         <v>30</v>
       </c>
       <c r="C37" t="s">
+        <v>226</v>
+      </c>
+      <c r="D37" t="s">
         <v>227</v>
       </c>
-      <c r="D37" t="s">
-        <v>228</v>
-      </c>
       <c r="E37" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F37" t="s">
         <v>106</v>
       </c>
       <c r="G37" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="J37" t="s">
         <v>83</v>
@@ -3572,19 +3572,19 @@
         <v>30</v>
       </c>
       <c r="C38" t="s">
+        <v>229</v>
+      </c>
+      <c r="D38" t="s">
         <v>230</v>
       </c>
-      <c r="D38" t="s">
+      <c r="E38" t="s">
         <v>231</v>
-      </c>
-      <c r="E38" t="s">
-        <v>232</v>
       </c>
       <c r="F38" t="s">
         <v>106</v>
       </c>
       <c r="G38" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="J38" t="s">
         <v>83</v>
@@ -3610,19 +3610,19 @@
         <v>30</v>
       </c>
       <c r="C39" t="s">
+        <v>233</v>
+      </c>
+      <c r="D39" t="s">
         <v>234</v>
       </c>
-      <c r="D39" t="s">
+      <c r="E39" t="s">
         <v>235</v>
       </c>
-      <c r="E39" t="s">
+      <c r="F39" t="s">
+        <v>55</v>
+      </c>
+      <c r="I39" s="1" t="s">
         <v>236</v>
-      </c>
-      <c r="F39" t="s">
-        <v>55</v>
-      </c>
-      <c r="I39" s="1" t="s">
-        <v>237</v>
       </c>
       <c r="J39" t="s">
         <v>83</v>
@@ -3648,19 +3648,19 @@
         <v>30</v>
       </c>
       <c r="C40" t="s">
+        <v>237</v>
+      </c>
+      <c r="D40" t="s">
         <v>238</v>
       </c>
-      <c r="D40" t="s">
+      <c r="E40" t="s">
         <v>239</v>
-      </c>
-      <c r="E40" t="s">
-        <v>240</v>
       </c>
       <c r="F40" t="s">
         <v>106</v>
       </c>
       <c r="G40" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="J40" t="s">
         <v>83</v>
@@ -3686,19 +3686,19 @@
         <v>30</v>
       </c>
       <c r="C41" t="s">
+        <v>240</v>
+      </c>
+      <c r="D41" t="s">
         <v>241</v>
       </c>
-      <c r="D41" t="s">
+      <c r="E41" t="s">
         <v>242</v>
       </c>
-      <c r="E41" t="s">
-        <v>243</v>
-      </c>
       <c r="F41" t="s">
         <v>55</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J41" t="s">
         <v>83</v>
@@ -3724,19 +3724,19 @@
         <v>30</v>
       </c>
       <c r="C42" t="s">
+        <v>243</v>
+      </c>
+      <c r="D42" t="s">
         <v>244</v>
       </c>
-      <c r="D42" t="s">
-        <v>245</v>
-      </c>
       <c r="E42" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F42" t="s">
         <v>106</v>
       </c>
       <c r="G42" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="J42" t="s">
         <v>83</v>
@@ -3754,7 +3754,7 @@
         <v>84</v>
       </c>
       <c r="AA42" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="AB42" t="s">
         <v>41</v>
@@ -3768,31 +3768,31 @@
         <v>30</v>
       </c>
       <c r="C43" t="s">
+        <v>247</v>
+      </c>
+      <c r="D43" t="s">
         <v>248</v>
       </c>
-      <c r="D43" t="s">
+      <c r="E43" t="s">
         <v>249</v>
-      </c>
-      <c r="E43" t="s">
-        <v>250</v>
       </c>
       <c r="F43" t="s">
         <v>106</v>
       </c>
       <c r="G43" t="s">
+        <v>250</v>
+      </c>
+      <c r="J43" t="s">
         <v>251</v>
       </c>
-      <c r="J43" t="s">
+      <c r="K43" t="s">
         <v>252</v>
       </c>
-      <c r="K43" t="s">
+      <c r="Q43" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="Q43" s="1" t="s">
+      <c r="S43" s="1" t="s">
         <v>254</v>
-      </c>
-      <c r="S43" s="1" t="s">
-        <v>255</v>
       </c>
       <c r="T43" t="s">
         <v>36</v>
@@ -3804,10 +3804,10 @@
         <v>101</v>
       </c>
       <c r="W43" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="AA43" t="s">
         <v>256</v>
-      </c>
-      <c r="AA43" t="s">
-        <v>257</v>
       </c>
       <c r="AB43" t="s">
         <v>41</v>
@@ -3821,25 +3821,25 @@
         <v>30</v>
       </c>
       <c r="C44" t="s">
+        <v>257</v>
+      </c>
+      <c r="D44" t="s">
         <v>258</v>
       </c>
-      <c r="D44" t="s">
+      <c r="E44" t="s">
+        <v>258</v>
+      </c>
+      <c r="F44" t="s">
+        <v>55</v>
+      </c>
+      <c r="I44" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="E44" t="s">
-        <v>259</v>
-      </c>
-      <c r="F44" t="s">
-        <v>55</v>
-      </c>
-      <c r="I44" s="1" t="s">
+      <c r="J44" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="J44" s="1" t="s">
+      <c r="Q44" s="1" t="s">
         <v>261</v>
-      </c>
-      <c r="Q44" s="1" t="s">
-        <v>262</v>
       </c>
       <c r="T44" t="s">
         <v>36</v>
@@ -3851,7 +3851,7 @@
         <v>101</v>
       </c>
       <c r="W44" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="45" spans="1:28" ht="45" x14ac:dyDescent="0.25">
@@ -3862,19 +3862,19 @@
         <v>30</v>
       </c>
       <c r="C45" t="s">
+        <v>263</v>
+      </c>
+      <c r="D45" t="s">
         <v>264</v>
       </c>
-      <c r="D45" t="s">
+      <c r="E45" t="s">
         <v>265</v>
       </c>
-      <c r="E45" t="s">
+      <c r="F45" t="s">
+        <v>55</v>
+      </c>
+      <c r="I45" s="1" t="s">
         <v>266</v>
-      </c>
-      <c r="F45" t="s">
-        <v>55</v>
-      </c>
-      <c r="I45" s="1" t="s">
-        <v>267</v>
       </c>
       <c r="J45" t="s">
         <v>83</v>
@@ -3900,28 +3900,28 @@
         <v>30</v>
       </c>
       <c r="C46" t="s">
+        <v>267</v>
+      </c>
+      <c r="D46" t="s">
         <v>268</v>
       </c>
-      <c r="D46" t="s">
+      <c r="E46" t="s">
+        <v>268</v>
+      </c>
+      <c r="F46" t="s">
+        <v>55</v>
+      </c>
+      <c r="I46" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="E46" t="s">
-        <v>269</v>
-      </c>
-      <c r="F46" t="s">
-        <v>55</v>
-      </c>
-      <c r="I46" s="1" t="s">
+      <c r="J46" t="s">
         <v>270</v>
       </c>
-      <c r="J46" t="s">
+      <c r="K46" t="s">
         <v>271</v>
       </c>
-      <c r="K46" t="s">
+      <c r="Q46" s="1" t="s">
         <v>272</v>
-      </c>
-      <c r="Q46" s="1" t="s">
-        <v>273</v>
       </c>
       <c r="T46" t="s">
         <v>36</v>
@@ -3933,10 +3933,10 @@
         <v>59</v>
       </c>
       <c r="W46" t="s">
+        <v>273</v>
+      </c>
+      <c r="X46" s="1" t="s">
         <v>274</v>
-      </c>
-      <c r="X46" s="1" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="47" spans="1:28" ht="165" x14ac:dyDescent="0.25">
@@ -3947,25 +3947,25 @@
         <v>30</v>
       </c>
       <c r="C47" t="s">
+        <v>275</v>
+      </c>
+      <c r="D47" t="s">
         <v>276</v>
       </c>
-      <c r="D47" t="s">
+      <c r="E47" t="s">
+        <v>276</v>
+      </c>
+      <c r="F47" t="s">
+        <v>55</v>
+      </c>
+      <c r="G47" t="s">
         <v>277</v>
       </c>
-      <c r="E47" t="s">
-        <v>277</v>
-      </c>
-      <c r="F47" t="s">
-        <v>55</v>
-      </c>
-      <c r="G47" t="s">
+      <c r="J47" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="J47" s="1" t="s">
+      <c r="K47" s="1" t="s">
         <v>279</v>
-      </c>
-      <c r="K47" s="1" t="s">
-        <v>280</v>
       </c>
       <c r="T47" t="s">
         <v>36</v>
@@ -3977,7 +3977,7 @@
         <v>101</v>
       </c>
       <c r="W47" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="48" spans="1:28" ht="75" x14ac:dyDescent="0.25">
@@ -3988,28 +3988,28 @@
         <v>30</v>
       </c>
       <c r="C48" t="s">
+        <v>281</v>
+      </c>
+      <c r="D48" t="s">
         <v>282</v>
       </c>
-      <c r="D48" t="s">
+      <c r="E48" t="s">
+        <v>282</v>
+      </c>
+      <c r="F48" t="s">
+        <v>55</v>
+      </c>
+      <c r="I48" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="E48" t="s">
-        <v>283</v>
-      </c>
-      <c r="F48" t="s">
-        <v>55</v>
-      </c>
-      <c r="I48" s="1" t="s">
+      <c r="J48" t="s">
         <v>284</v>
       </c>
-      <c r="J48" t="s">
+      <c r="K48" t="s">
         <v>285</v>
       </c>
-      <c r="K48" t="s">
+      <c r="Q48" s="1" t="s">
         <v>286</v>
-      </c>
-      <c r="Q48" s="1" t="s">
-        <v>287</v>
       </c>
       <c r="T48" t="s">
         <v>36</v>
@@ -4021,7 +4021,7 @@
         <v>59</v>
       </c>
       <c r="W48" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="49" spans="1:28" ht="30" x14ac:dyDescent="0.25">
@@ -4032,19 +4032,19 @@
         <v>30</v>
       </c>
       <c r="C49" t="s">
+        <v>288</v>
+      </c>
+      <c r="D49" t="s">
         <v>289</v>
       </c>
-      <c r="D49" t="s">
+      <c r="E49" t="s">
         <v>290</v>
       </c>
-      <c r="E49" t="s">
+      <c r="F49" t="s">
+        <v>55</v>
+      </c>
+      <c r="I49" s="1" t="s">
         <v>291</v>
-      </c>
-      <c r="F49" t="s">
-        <v>55</v>
-      </c>
-      <c r="I49" s="1" t="s">
-        <v>292</v>
       </c>
       <c r="J49" t="s">
         <v>83</v>
@@ -4070,19 +4070,19 @@
         <v>30</v>
       </c>
       <c r="C50" t="s">
+        <v>292</v>
+      </c>
+      <c r="D50" t="s">
         <v>293</v>
       </c>
-      <c r="D50" t="s">
+      <c r="E50" t="s">
         <v>294</v>
       </c>
-      <c r="E50" t="s">
-        <v>295</v>
-      </c>
       <c r="F50" t="s">
         <v>55</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J50" t="s">
         <v>83</v>
@@ -4108,19 +4108,19 @@
         <v>30</v>
       </c>
       <c r="C51" t="s">
+        <v>295</v>
+      </c>
+      <c r="D51" t="s">
         <v>296</v>
       </c>
-      <c r="D51" t="s">
-        <v>297</v>
-      </c>
       <c r="E51" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F51" t="s">
         <v>55</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J51" t="s">
         <v>83</v>
@@ -4146,19 +4146,19 @@
         <v>30</v>
       </c>
       <c r="C52" t="s">
+        <v>297</v>
+      </c>
+      <c r="D52" t="s">
         <v>298</v>
       </c>
-      <c r="D52" t="s">
+      <c r="E52" t="s">
+        <v>298</v>
+      </c>
+      <c r="F52" t="s">
+        <v>55</v>
+      </c>
+      <c r="I52" s="1" t="s">
         <v>299</v>
-      </c>
-      <c r="E52" t="s">
-        <v>299</v>
-      </c>
-      <c r="F52" t="s">
-        <v>55</v>
-      </c>
-      <c r="I52" s="1" t="s">
-        <v>300</v>
       </c>
       <c r="J52" t="s">
         <v>83</v>
@@ -4184,19 +4184,19 @@
         <v>30</v>
       </c>
       <c r="C53" t="s">
+        <v>300</v>
+      </c>
+      <c r="D53" t="s">
         <v>301</v>
       </c>
-      <c r="D53" t="s">
-        <v>302</v>
-      </c>
       <c r="E53" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="F53" t="s">
         <v>55</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J53" t="s">
         <v>83</v>
@@ -4222,19 +4222,19 @@
         <v>30</v>
       </c>
       <c r="C54" t="s">
+        <v>302</v>
+      </c>
+      <c r="D54" t="s">
         <v>303</v>
       </c>
-      <c r="D54" t="s">
-        <v>304</v>
-      </c>
       <c r="E54" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F54" t="s">
         <v>55</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J54" t="s">
         <v>83</v>
@@ -4260,19 +4260,19 @@
         <v>30</v>
       </c>
       <c r="C55" t="s">
+        <v>304</v>
+      </c>
+      <c r="D55" t="s">
         <v>305</v>
       </c>
-      <c r="D55" t="s">
-        <v>306</v>
-      </c>
       <c r="E55" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F55" t="s">
         <v>55</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J55" t="s">
         <v>83</v>
@@ -4298,19 +4298,19 @@
         <v>30</v>
       </c>
       <c r="C56" t="s">
+        <v>306</v>
+      </c>
+      <c r="D56" t="s">
         <v>307</v>
       </c>
-      <c r="D56" t="s">
-        <v>308</v>
-      </c>
       <c r="E56" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F56" t="s">
         <v>55</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J56" t="s">
         <v>83</v>
@@ -4328,7 +4328,7 @@
         <v>84</v>
       </c>
       <c r="AA56" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AB56" t="s">
         <v>41</v>
@@ -4342,19 +4342,19 @@
         <v>30</v>
       </c>
       <c r="C57" t="s">
+        <v>309</v>
+      </c>
+      <c r="D57" t="s">
         <v>310</v>
       </c>
-      <c r="D57" t="s">
-        <v>311</v>
-      </c>
       <c r="E57" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F57" t="s">
         <v>55</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J57" t="s">
         <v>83</v>
@@ -4380,19 +4380,19 @@
         <v>30</v>
       </c>
       <c r="C58" t="s">
+        <v>311</v>
+      </c>
+      <c r="D58" t="s">
         <v>312</v>
       </c>
-      <c r="D58" t="s">
+      <c r="E58" t="s">
         <v>313</v>
       </c>
-      <c r="E58" t="s">
-        <v>314</v>
-      </c>
       <c r="F58" t="s">
         <v>55</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J58" t="s">
         <v>83</v>
@@ -4418,13 +4418,13 @@
         <v>30</v>
       </c>
       <c r="C59" t="s">
+        <v>314</v>
+      </c>
+      <c r="D59" t="s">
         <v>315</v>
       </c>
-      <c r="D59" t="s">
-        <v>316</v>
-      </c>
       <c r="E59" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F59" t="s">
         <v>55</v>
@@ -4453,13 +4453,13 @@
         <v>30</v>
       </c>
       <c r="C60" t="s">
+        <v>316</v>
+      </c>
+      <c r="D60" t="s">
         <v>317</v>
       </c>
-      <c r="D60" t="s">
-        <v>318</v>
-      </c>
       <c r="E60" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F60" t="s">
         <v>55</v>
@@ -4488,13 +4488,13 @@
         <v>30</v>
       </c>
       <c r="C61" t="s">
+        <v>318</v>
+      </c>
+      <c r="D61" t="s">
         <v>319</v>
       </c>
-      <c r="D61" t="s">
-        <v>320</v>
-      </c>
       <c r="E61" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F61" t="s">
         <v>55</v>
@@ -4523,13 +4523,13 @@
         <v>30</v>
       </c>
       <c r="C62" t="s">
+        <v>320</v>
+      </c>
+      <c r="D62" t="s">
         <v>321</v>
       </c>
-      <c r="D62" t="s">
-        <v>322</v>
-      </c>
       <c r="E62" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="F62" t="s">
         <v>55</v>
@@ -4558,13 +4558,13 @@
         <v>30</v>
       </c>
       <c r="C63" t="s">
+        <v>322</v>
+      </c>
+      <c r="D63" t="s">
         <v>323</v>
       </c>
-      <c r="D63" t="s">
-        <v>324</v>
-      </c>
       <c r="E63" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="F63" t="s">
         <v>55</v>
@@ -4593,13 +4593,13 @@
         <v>30</v>
       </c>
       <c r="C64" t="s">
+        <v>324</v>
+      </c>
+      <c r="D64" t="s">
         <v>325</v>
       </c>
-      <c r="D64" t="s">
-        <v>326</v>
-      </c>
       <c r="E64" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="F64" t="s">
         <v>55</v>
@@ -4628,13 +4628,13 @@
         <v>30</v>
       </c>
       <c r="C65" t="s">
+        <v>326</v>
+      </c>
+      <c r="D65" t="s">
         <v>327</v>
       </c>
-      <c r="D65" t="s">
-        <v>328</v>
-      </c>
       <c r="E65" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="F65" t="s">
         <v>55</v>
@@ -4663,19 +4663,19 @@
         <v>30</v>
       </c>
       <c r="C66" t="s">
+        <v>328</v>
+      </c>
+      <c r="D66" t="s">
         <v>329</v>
       </c>
-      <c r="D66" t="s">
+      <c r="E66" t="s">
+        <v>329</v>
+      </c>
+      <c r="F66" t="s">
+        <v>55</v>
+      </c>
+      <c r="I66" s="1" t="s">
         <v>330</v>
-      </c>
-      <c r="E66" t="s">
-        <v>330</v>
-      </c>
-      <c r="F66" t="s">
-        <v>55</v>
-      </c>
-      <c r="I66" s="1" t="s">
-        <v>331</v>
       </c>
       <c r="J66" t="s">
         <v>83</v>
@@ -4701,19 +4701,19 @@
         <v>30</v>
       </c>
       <c r="C67" t="s">
+        <v>331</v>
+      </c>
+      <c r="D67" t="s">
         <v>332</v>
       </c>
-      <c r="D67" t="s">
-        <v>333</v>
-      </c>
       <c r="E67" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="F67" t="s">
         <v>106</v>
       </c>
       <c r="G67" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="J67" t="s">
         <v>83</v>
@@ -4739,19 +4739,19 @@
         <v>30</v>
       </c>
       <c r="C68" t="s">
+        <v>334</v>
+      </c>
+      <c r="D68" t="s">
         <v>335</v>
       </c>
-      <c r="D68" t="s">
+      <c r="E68" t="s">
+        <v>335</v>
+      </c>
+      <c r="F68" t="s">
+        <v>55</v>
+      </c>
+      <c r="I68" s="1" t="s">
         <v>336</v>
-      </c>
-      <c r="E68" t="s">
-        <v>336</v>
-      </c>
-      <c r="F68" t="s">
-        <v>55</v>
-      </c>
-      <c r="I68" s="1" t="s">
-        <v>337</v>
       </c>
       <c r="J68" t="s">
         <v>83</v>
@@ -4777,22 +4777,22 @@
         <v>30</v>
       </c>
       <c r="C69" t="s">
+        <v>337</v>
+      </c>
+      <c r="D69" t="s">
         <v>338</v>
       </c>
-      <c r="D69" t="s">
+      <c r="E69" t="s">
+        <v>338</v>
+      </c>
+      <c r="F69" t="s">
+        <v>55</v>
+      </c>
+      <c r="I69" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="E69" t="s">
-        <v>339</v>
-      </c>
-      <c r="F69" t="s">
-        <v>55</v>
-      </c>
-      <c r="I69" s="1" t="s">
+      <c r="J69" t="s">
         <v>340</v>
-      </c>
-      <c r="J69" t="s">
-        <v>341</v>
       </c>
       <c r="T69" t="s">
         <v>36</v>
@@ -4807,7 +4807,7 @@
         <v>47</v>
       </c>
       <c r="X69" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="70" spans="1:24" ht="180" x14ac:dyDescent="0.25">
@@ -4818,28 +4818,28 @@
         <v>30</v>
       </c>
       <c r="C70" t="s">
+        <v>342</v>
+      </c>
+      <c r="D70" t="s">
         <v>343</v>
       </c>
-      <c r="D70" t="s">
+      <c r="E70" t="s">
+        <v>343</v>
+      </c>
+      <c r="F70" t="s">
+        <v>55</v>
+      </c>
+      <c r="I70" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="E70" t="s">
-        <v>344</v>
-      </c>
-      <c r="F70" t="s">
-        <v>55</v>
-      </c>
-      <c r="I70" s="1" t="s">
+      <c r="J70" s="1" t="s">
         <v>345</v>
       </c>
-      <c r="J70" s="1" t="s">
+      <c r="K70" t="s">
         <v>346</v>
       </c>
-      <c r="K70" t="s">
+      <c r="M70" s="1" t="s">
         <v>347</v>
-      </c>
-      <c r="M70" s="1" t="s">
-        <v>348</v>
       </c>
       <c r="T70" t="s">
         <v>36</v>
@@ -4851,7 +4851,7 @@
         <v>101</v>
       </c>
       <c r="W70" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="71" spans="1:24" ht="90" x14ac:dyDescent="0.25">
@@ -4862,28 +4862,28 @@
         <v>30</v>
       </c>
       <c r="C71" t="s">
+        <v>349</v>
+      </c>
+      <c r="D71" t="s">
         <v>350</v>
       </c>
-      <c r="D71" t="s">
+      <c r="E71" t="s">
+        <v>350</v>
+      </c>
+      <c r="F71" t="s">
+        <v>55</v>
+      </c>
+      <c r="I71" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="J71" t="s">
         <v>351</v>
       </c>
-      <c r="E71" t="s">
-        <v>351</v>
-      </c>
-      <c r="F71" t="s">
-        <v>55</v>
-      </c>
-      <c r="I71" s="1" t="s">
-        <v>345</v>
-      </c>
-      <c r="J71" t="s">
+      <c r="K71" t="s">
+        <v>346</v>
+      </c>
+      <c r="M71" s="1" t="s">
         <v>352</v>
-      </c>
-      <c r="K71" t="s">
-        <v>347</v>
-      </c>
-      <c r="M71" s="1" t="s">
-        <v>353</v>
       </c>
       <c r="T71" t="s">
         <v>36</v>
@@ -4895,7 +4895,7 @@
         <v>101</v>
       </c>
       <c r="W71" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="72" spans="1:24" ht="90" x14ac:dyDescent="0.25">
@@ -4906,28 +4906,28 @@
         <v>30</v>
       </c>
       <c r="C72" t="s">
+        <v>354</v>
+      </c>
+      <c r="D72" t="s">
         <v>355</v>
       </c>
-      <c r="D72" t="s">
+      <c r="E72" t="s">
+        <v>355</v>
+      </c>
+      <c r="F72" t="s">
+        <v>55</v>
+      </c>
+      <c r="I72" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="J72" t="s">
         <v>356</v>
       </c>
-      <c r="E72" t="s">
-        <v>356</v>
-      </c>
-      <c r="F72" t="s">
-        <v>55</v>
-      </c>
-      <c r="I72" s="1" t="s">
-        <v>345</v>
-      </c>
-      <c r="J72" t="s">
+      <c r="K72" t="s">
+        <v>346</v>
+      </c>
+      <c r="M72" s="1" t="s">
         <v>357</v>
-      </c>
-      <c r="K72" t="s">
-        <v>347</v>
-      </c>
-      <c r="M72" s="1" t="s">
-        <v>358</v>
       </c>
       <c r="T72" t="s">
         <v>36</v>
@@ -4939,7 +4939,7 @@
         <v>101</v>
       </c>
       <c r="W72" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="73" spans="1:24" ht="165" x14ac:dyDescent="0.25">
@@ -4950,37 +4950,37 @@
         <v>30</v>
       </c>
       <c r="C73" t="s">
+        <v>359</v>
+      </c>
+      <c r="D73" t="s">
         <v>360</v>
       </c>
-      <c r="D73" t="s">
+      <c r="E73" t="s">
         <v>361</v>
       </c>
-      <c r="E73" t="s">
+      <c r="F73" t="s">
+        <v>55</v>
+      </c>
+      <c r="I73" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="F73" t="s">
-        <v>55</v>
-      </c>
-      <c r="I73" s="1" t="s">
+      <c r="J73" s="1" t="s">
         <v>363</v>
       </c>
-      <c r="J73" s="1" t="s">
+      <c r="T73" t="s">
+        <v>84</v>
+      </c>
+      <c r="U73" t="s">
+        <v>206</v>
+      </c>
+      <c r="V73" t="s">
+        <v>84</v>
+      </c>
+      <c r="W73" t="s">
+        <v>84</v>
+      </c>
+      <c r="X73" t="s">
         <v>364</v>
-      </c>
-      <c r="T73" t="s">
-        <v>84</v>
-      </c>
-      <c r="U73" t="s">
-        <v>207</v>
-      </c>
-      <c r="V73" t="s">
-        <v>84</v>
-      </c>
-      <c r="W73" t="s">
-        <v>84</v>
-      </c>
-      <c r="X73" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="74" spans="1:24" ht="210" x14ac:dyDescent="0.25">
@@ -4991,28 +4991,28 @@
         <v>30</v>
       </c>
       <c r="C74" t="s">
+        <v>365</v>
+      </c>
+      <c r="D74" t="s">
         <v>366</v>
       </c>
-      <c r="D74" t="s">
+      <c r="E74" t="s">
         <v>367</v>
       </c>
-      <c r="E74" t="s">
+      <c r="F74" t="s">
+        <v>55</v>
+      </c>
+      <c r="I74" s="1" t="s">
         <v>368</v>
       </c>
-      <c r="F74" t="s">
-        <v>55</v>
-      </c>
-      <c r="I74" s="1" t="s">
+      <c r="J74" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="K74" t="s">
         <v>369</v>
       </c>
-      <c r="J74" s="1" t="s">
-        <v>364</v>
-      </c>
-      <c r="K74" t="s">
-        <v>370</v>
-      </c>
       <c r="M74" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="T74" t="s">
         <v>36</v>
@@ -5024,7 +5024,7 @@
         <v>101</v>
       </c>
       <c r="W74" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="75" spans="1:24" ht="195" x14ac:dyDescent="0.25">
@@ -5035,28 +5035,28 @@
         <v>30</v>
       </c>
       <c r="C75" t="s">
+        <v>371</v>
+      </c>
+      <c r="D75" t="s">
         <v>372</v>
       </c>
-      <c r="D75" t="s">
+      <c r="E75" t="s">
         <v>373</v>
       </c>
-      <c r="E75" t="s">
+      <c r="F75" t="s">
+        <v>55</v>
+      </c>
+      <c r="I75" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="F75" t="s">
-        <v>55</v>
-      </c>
-      <c r="I75" s="1" t="s">
+      <c r="J75" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="J75" s="1" t="s">
+      <c r="K75" t="s">
         <v>376</v>
       </c>
-      <c r="K75" t="s">
-        <v>377</v>
-      </c>
       <c r="M75" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="T75" t="s">
         <v>36</v>
@@ -5068,7 +5068,7 @@
         <v>101</v>
       </c>
       <c r="W75" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="76" spans="1:24" ht="409.5" x14ac:dyDescent="0.25">
@@ -5079,28 +5079,28 @@
         <v>30</v>
       </c>
       <c r="C76" t="s">
+        <v>378</v>
+      </c>
+      <c r="D76" t="s">
         <v>379</v>
       </c>
-      <c r="D76" t="s">
+      <c r="E76" t="s">
         <v>380</v>
       </c>
-      <c r="E76" t="s">
+      <c r="F76" t="s">
+        <v>55</v>
+      </c>
+      <c r="G76" t="s">
+        <v>333</v>
+      </c>
+      <c r="J76" t="s">
         <v>381</v>
       </c>
-      <c r="F76" t="s">
-        <v>55</v>
-      </c>
-      <c r="G76" t="s">
-        <v>334</v>
-      </c>
-      <c r="J76" t="s">
+      <c r="K76" s="1" t="s">
         <v>382</v>
       </c>
-      <c r="K76" s="1" t="s">
+      <c r="Q76" t="s">
         <v>383</v>
-      </c>
-      <c r="Q76" t="s">
-        <v>384</v>
       </c>
       <c r="T76" t="s">
         <v>36</v>
@@ -5109,13 +5109,13 @@
         <v>73</v>
       </c>
       <c r="V76" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="W76" t="s">
+        <v>384</v>
+      </c>
+      <c r="X76" s="1" t="s">
         <v>385</v>
-      </c>
-      <c r="X76" s="1" t="s">
-        <v>386</v>
       </c>
     </row>
     <row r="77" spans="1:24" ht="195" x14ac:dyDescent="0.25">
@@ -5126,28 +5126,28 @@
         <v>30</v>
       </c>
       <c r="C77" t="s">
+        <v>386</v>
+      </c>
+      <c r="D77" t="s">
         <v>387</v>
       </c>
-      <c r="D77" t="s">
+      <c r="E77" t="s">
         <v>388</v>
       </c>
-      <c r="E77" t="s">
+      <c r="F77" t="s">
+        <v>55</v>
+      </c>
+      <c r="I77" s="1" t="s">
         <v>389</v>
       </c>
-      <c r="F77" t="s">
-        <v>55</v>
-      </c>
-      <c r="I77" s="1" t="s">
+      <c r="J77" t="s">
+        <v>381</v>
+      </c>
+      <c r="K77" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="J77" t="s">
-        <v>382</v>
-      </c>
-      <c r="K77" s="1" t="s">
-        <v>391</v>
-      </c>
       <c r="Q77" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="T77" t="s">
         <v>36</v>
@@ -5159,7 +5159,7 @@
         <v>101</v>
       </c>
       <c r="W77" s="1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="78" spans="1:24" ht="45" x14ac:dyDescent="0.25">
@@ -5170,19 +5170,19 @@
         <v>30</v>
       </c>
       <c r="C78" t="s">
+        <v>392</v>
+      </c>
+      <c r="D78" t="s">
         <v>393</v>
       </c>
-      <c r="D78" t="s">
+      <c r="E78" t="s">
         <v>394</v>
       </c>
-      <c r="E78" t="s">
+      <c r="F78" t="s">
+        <v>55</v>
+      </c>
+      <c r="I78" s="1" t="s">
         <v>395</v>
-      </c>
-      <c r="F78" t="s">
-        <v>55</v>
-      </c>
-      <c r="I78" s="1" t="s">
-        <v>396</v>
       </c>
       <c r="J78" t="s">
         <v>83</v>
@@ -5208,19 +5208,19 @@
         <v>30</v>
       </c>
       <c r="C79" t="s">
+        <v>396</v>
+      </c>
+      <c r="D79" t="s">
         <v>397</v>
       </c>
-      <c r="D79" t="s">
+      <c r="E79" t="s">
+        <v>397</v>
+      </c>
+      <c r="F79" t="s">
+        <v>55</v>
+      </c>
+      <c r="I79" s="1" t="s">
         <v>398</v>
-      </c>
-      <c r="E79" t="s">
-        <v>398</v>
-      </c>
-      <c r="F79" t="s">
-        <v>55</v>
-      </c>
-      <c r="I79" s="1" t="s">
-        <v>399</v>
       </c>
       <c r="J79" t="s">
         <v>83</v>
@@ -5246,19 +5246,19 @@
         <v>30</v>
       </c>
       <c r="C80" t="s">
+        <v>399</v>
+      </c>
+      <c r="D80" t="s">
         <v>400</v>
       </c>
-      <c r="D80" t="s">
+      <c r="E80" t="s">
         <v>401</v>
       </c>
-      <c r="E80" t="s">
-        <v>402</v>
-      </c>
       <c r="F80" t="s">
         <v>55</v>
       </c>
       <c r="I80" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J80" t="s">
         <v>83</v>
@@ -5284,19 +5284,19 @@
         <v>30</v>
       </c>
       <c r="C81" t="s">
+        <v>402</v>
+      </c>
+      <c r="D81" t="s">
         <v>403</v>
       </c>
-      <c r="D81" t="s">
+      <c r="E81" t="s">
         <v>404</v>
       </c>
-      <c r="E81" t="s">
-        <v>405</v>
-      </c>
       <c r="F81" t="s">
         <v>55</v>
       </c>
       <c r="I81" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J81" t="s">
         <v>83</v>
@@ -5322,19 +5322,19 @@
         <v>30</v>
       </c>
       <c r="C82" t="s">
+        <v>405</v>
+      </c>
+      <c r="D82" t="s">
         <v>406</v>
       </c>
-      <c r="D82" t="s">
+      <c r="E82" t="s">
         <v>407</v>
       </c>
-      <c r="E82" t="s">
-        <v>408</v>
-      </c>
       <c r="F82" t="s">
         <v>55</v>
       </c>
       <c r="I82" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J82" t="s">
         <v>83</v>
@@ -5360,13 +5360,13 @@
         <v>30</v>
       </c>
       <c r="C83" t="s">
+        <v>408</v>
+      </c>
+      <c r="D83" t="s">
         <v>409</v>
       </c>
-      <c r="D83" t="s">
+      <c r="E83" t="s">
         <v>410</v>
-      </c>
-      <c r="E83" t="s">
-        <v>411</v>
       </c>
       <c r="F83" t="s">
         <v>55</v>
@@ -5395,19 +5395,19 @@
         <v>30</v>
       </c>
       <c r="C84" t="s">
+        <v>411</v>
+      </c>
+      <c r="D84" t="s">
         <v>412</v>
       </c>
-      <c r="D84" t="s">
+      <c r="E84" t="s">
         <v>413</v>
       </c>
-      <c r="E84" t="s">
+      <c r="F84" t="s">
+        <v>55</v>
+      </c>
+      <c r="G84" t="s">
         <v>414</v>
-      </c>
-      <c r="F84" t="s">
-        <v>55</v>
-      </c>
-      <c r="G84" t="s">
-        <v>415</v>
       </c>
       <c r="J84" t="s">
         <v>83</v>

</xml_diff>